<commit_message>
Prime 1 à 4 de fait
</commit_message>
<xml_diff>
--- a/Excel_Exercice04_OperateursFonctionsCond.xlsx
+++ b/Excel_Exercice04_OperateursFonctionsCond.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilio\OneDrive\Bureau\École\Programmation\Outils et gestion\Remise-C13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92EC117-7FDE-410F-99D1-9E966F25DD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2066A0EF-DB93-4572-A021-4BE7C8D294A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -288,8 +288,64 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Laurentiu Dilion</author>
+  </authors>
+  <commentList>
+    <comment ref="U7" authorId="0" shapeId="0" xr:uid="{96A6E7DA-6286-4901-A6F5-C5FA11A87EF4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jean-Christophe Dermers</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="70">
   <si>
     <t>Ventes réalisées</t>
   </si>
@@ -574,6 +630,9 @@
       <t>S</t>
     </r>
   </si>
+  <si>
+    <t>Oui</t>
+  </si>
 </sst>
 </file>
 
@@ -583,9 +642,9 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -767,8 +826,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -877,8 +949,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="50">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -1437,11 +1521,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -1747,9 +1891,137 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -1866,170 +2138,169 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD6DCFA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDDEBFB"/>
+      <color rgb="FFD6DCFA"/>
+      <color rgb="FFD6DEFA"/>
       <color rgb="FFECF2F8"/>
       <color rgb="FFF1EFF5"/>
       <color rgb="FFF8EDEC"/>
@@ -2044,6 +2315,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2369,7 +2644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="91" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="N1" zoomScale="112" workbookViewId="0">
       <selection activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
@@ -2397,41 +2672,41 @@
   <sheetData>
     <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:34" ht="19.2" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="132" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
-      <c r="S2" s="100"/>
-      <c r="T2" s="100"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="100"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="100"/>
-      <c r="Z2" s="100"/>
-      <c r="AA2" s="100"/>
-      <c r="AB2" s="100"/>
-      <c r="AC2" s="100"/>
-      <c r="AD2" s="100"/>
-      <c r="AE2" s="100"/>
-      <c r="AF2" s="100"/>
-      <c r="AG2" s="100"/>
-      <c r="AH2" s="100"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
+      <c r="M2" s="132"/>
+      <c r="N2" s="132"/>
+      <c r="O2" s="132"/>
+      <c r="P2" s="132"/>
+      <c r="Q2" s="132"/>
+      <c r="R2" s="132"/>
+      <c r="S2" s="132"/>
+      <c r="T2" s="132"/>
+      <c r="U2" s="132"/>
+      <c r="V2" s="132"/>
+      <c r="W2" s="132"/>
+      <c r="X2" s="132"/>
+      <c r="Y2" s="132"/>
+      <c r="Z2" s="132"/>
+      <c r="AA2" s="132"/>
+      <c r="AB2" s="132"/>
+      <c r="AC2" s="132"/>
+      <c r="AD2" s="132"/>
+      <c r="AE2" s="132"/>
+      <c r="AF2" s="132"/>
+      <c r="AG2" s="132"/>
+      <c r="AH2" s="132"/>
     </row>
     <row r="3" spans="2:34" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -2442,122 +2717,122 @@
     </row>
     <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
-      <c r="L5" s="102" t="s">
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="L5" s="134" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="102"/>
-      <c r="N5" s="102"/>
-      <c r="O5" s="102"/>
-      <c r="P5" s="102"/>
-      <c r="R5" s="103" t="s">
+      <c r="M5" s="134"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
+      <c r="R5" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="103"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="103"/>
-      <c r="X5" s="103"/>
-      <c r="Y5" s="103"/>
-      <c r="Z5" s="103"/>
-      <c r="AA5" s="103"/>
-      <c r="AB5" s="103"/>
-      <c r="AC5" s="103"/>
-      <c r="AD5" s="103"/>
-      <c r="AE5" s="103"/>
-      <c r="AF5" s="103"/>
-      <c r="AG5" s="103"/>
-      <c r="AH5" s="103"/>
+      <c r="S5" s="135"/>
+      <c r="T5" s="135"/>
+      <c r="U5" s="135"/>
+      <c r="V5" s="135"/>
+      <c r="W5" s="135"/>
+      <c r="X5" s="135"/>
+      <c r="Y5" s="135"/>
+      <c r="Z5" s="135"/>
+      <c r="AA5" s="135"/>
+      <c r="AB5" s="135"/>
+      <c r="AC5" s="135"/>
+      <c r="AD5" s="135"/>
+      <c r="AE5" s="135"/>
+      <c r="AF5" s="135"/>
+      <c r="AG5" s="135"/>
+      <c r="AH5" s="135"/>
     </row>
     <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="112" t="s">
+      <c r="D7" s="144" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="107"/>
-      <c r="I7" s="87" t="s">
+      <c r="H7" s="139"/>
+      <c r="I7" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="88"/>
+      <c r="J7" s="120"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="108" t="s">
+      <c r="L7" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="109"/>
-      <c r="N7" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="109"/>
-      <c r="P7" s="96" t="s">
+      <c r="M7" s="141"/>
+      <c r="N7" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="141"/>
+      <c r="P7" s="128" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="89" t="s">
+      <c r="R7" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="90"/>
+      <c r="S7" s="122"/>
       <c r="T7" s="11"/>
-      <c r="U7" s="89" t="s">
+      <c r="U7" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="90"/>
-      <c r="W7" s="89" t="s">
+      <c r="V7" s="122"/>
+      <c r="W7" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="90"/>
-      <c r="Y7" s="89" t="s">
+      <c r="X7" s="122"/>
+      <c r="Y7" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="90"/>
-      <c r="AA7" s="89" t="s">
+      <c r="Z7" s="122"/>
+      <c r="AA7" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="90"/>
-      <c r="AC7" s="89" t="s">
+      <c r="AB7" s="122"/>
+      <c r="AC7" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="90"/>
-      <c r="AE7" s="89" t="s">
+      <c r="AD7" s="122"/>
+      <c r="AE7" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="90"/>
+      <c r="AF7" s="122"/>
       <c r="AG7" s="11"/>
-      <c r="AH7" s="98" t="s">
+      <c r="AH7" s="130" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="95"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="115"/>
+      <c r="B8" s="127"/>
+      <c r="C8" s="143"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="147"/>
       <c r="G8" s="13" t="s">
         <v>9</v>
       </c>
@@ -2583,7 +2858,7 @@
       <c r="O8" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="97"/>
+      <c r="P8" s="129"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="20" t="s">
         <v>9</v>
@@ -2629,7 +2904,7 @@
         <v>40</v>
       </c>
       <c r="AG8" s="12"/>
-      <c r="AH8" s="99"/>
+      <c r="AH8" s="131"/>
     </row>
     <row r="9" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="37" t="s">
@@ -4633,46 +4908,46 @@
       <c r="AH28" s="4"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B29" s="91" t="s">
+      <c r="B29" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="92"/>
-      <c r="D29" s="93"/>
-      <c r="E29" s="91" t="s">
+      <c r="C29" s="124"/>
+      <c r="D29" s="125"/>
+      <c r="E29" s="123" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="93"/>
-      <c r="G29" s="91" t="s">
+      <c r="F29" s="125"/>
+      <c r="G29" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="92"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="92"/>
-      <c r="M29" s="92"/>
-      <c r="N29" s="92"/>
-      <c r="O29" s="92"/>
-      <c r="P29" s="93"/>
-      <c r="R29" s="91" t="s">
+      <c r="H29" s="124"/>
+      <c r="I29" s="124"/>
+      <c r="J29" s="124"/>
+      <c r="K29" s="124"/>
+      <c r="L29" s="124"/>
+      <c r="M29" s="124"/>
+      <c r="N29" s="124"/>
+      <c r="O29" s="124"/>
+      <c r="P29" s="125"/>
+      <c r="R29" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="92"/>
-      <c r="T29" s="92"/>
-      <c r="U29" s="92"/>
-      <c r="V29" s="92"/>
-      <c r="W29" s="92"/>
-      <c r="X29" s="92"/>
-      <c r="Y29" s="92"/>
-      <c r="Z29" s="92"/>
-      <c r="AA29" s="92"/>
-      <c r="AB29" s="92"/>
-      <c r="AC29" s="92"/>
-      <c r="AD29" s="92"/>
-      <c r="AE29" s="92"/>
-      <c r="AF29" s="92"/>
-      <c r="AG29" s="92"/>
-      <c r="AH29" s="93"/>
+      <c r="S29" s="124"/>
+      <c r="T29" s="124"/>
+      <c r="U29" s="124"/>
+      <c r="V29" s="124"/>
+      <c r="W29" s="124"/>
+      <c r="X29" s="124"/>
+      <c r="Y29" s="124"/>
+      <c r="Z29" s="124"/>
+      <c r="AA29" s="124"/>
+      <c r="AB29" s="124"/>
+      <c r="AC29" s="124"/>
+      <c r="AD29" s="124"/>
+      <c r="AE29" s="124"/>
+      <c r="AF29" s="124"/>
+      <c r="AG29" s="124"/>
+      <c r="AH29" s="125"/>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="E31" s="8"/>
@@ -5022,11 +5297,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AH33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="AD23" sqref="AD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -5039,949 +5314,1784 @@
     <col min="6" max="6" width="14.42578125" style="85" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="85"/>
     <col min="8" max="8" width="11.28515625" style="85" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="85" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="85" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" style="85" customWidth="1"/>
-    <col min="12" max="16" width="10.7109375" style="85"/>
+    <col min="9" max="9" width="16.140625" style="85" customWidth="1"/>
+    <col min="10" max="10" width="16" style="85" customWidth="1"/>
+    <col min="11" max="11" width="1.140625" style="85" customWidth="1"/>
+    <col min="12" max="13" width="10.7109375" style="85"/>
+    <col min="14" max="14" width="15" style="85" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="85" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="85" customWidth="1"/>
     <col min="17" max="17" width="2" style="85" customWidth="1"/>
-    <col min="18" max="16384" width="10.7109375" style="85"/>
+    <col min="18" max="18" width="18.85546875" style="85" customWidth="1"/>
+    <col min="19" max="19" width="18" style="85" customWidth="1"/>
+    <col min="20" max="20" width="1" style="85" customWidth="1"/>
+    <col min="21" max="32" width="10.7109375" style="85"/>
+    <col min="33" max="33" width="1.5703125" style="85" customWidth="1"/>
+    <col min="34" max="34" width="18" style="85" customWidth="1"/>
+    <col min="35" max="16384" width="10.7109375" style="85"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:34" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="120" t="s">
+    <row r="2" spans="1:34" s="102" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="121"/>
-      <c r="Q2" s="121"/>
-      <c r="R2" s="121"/>
-      <c r="S2" s="121"/>
-      <c r="T2" s="121"/>
-      <c r="U2" s="121"/>
-      <c r="V2" s="121"/>
-      <c r="W2" s="121"/>
-      <c r="X2" s="121"/>
-      <c r="Y2" s="121"/>
-      <c r="Z2" s="121"/>
-      <c r="AA2" s="121"/>
-      <c r="AB2" s="121"/>
-      <c r="AC2" s="121"/>
-      <c r="AD2" s="121"/>
-      <c r="AE2" s="121"/>
-      <c r="AF2" s="121"/>
-      <c r="AG2" s="121"/>
-      <c r="AH2" s="121"/>
-    </row>
-    <row r="3" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="123" t="s">
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
+      <c r="Y2" s="104"/>
+      <c r="Z2" s="104"/>
+      <c r="AA2" s="104"/>
+      <c r="AB2" s="104"/>
+      <c r="AC2" s="104"/>
+      <c r="AD2" s="104"/>
+      <c r="AE2" s="104"/>
+      <c r="AF2" s="104"/>
+      <c r="AG2" s="104"/>
+      <c r="AH2" s="104"/>
+    </row>
+    <row r="3" spans="1:34" s="102" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="105" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="122"/>
-    </row>
-    <row r="5" spans="1:34" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="127" t="s">
+    <row r="4" spans="1:34" s="102" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="106"/>
+    </row>
+    <row r="5" spans="1:34" ht="16.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
-      <c r="L5" s="128" t="s">
+      <c r="C5" s="155"/>
+      <c r="D5" s="155"/>
+      <c r="E5" s="155"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="155"/>
+      <c r="J5" s="155"/>
+      <c r="L5" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="125"/>
-      <c r="N5" s="125"/>
-      <c r="O5" s="125"/>
-      <c r="P5" s="125"/>
-      <c r="R5" s="129" t="s">
+      <c r="M5" s="157"/>
+      <c r="N5" s="157"/>
+      <c r="O5" s="157"/>
+      <c r="P5" s="157"/>
+      <c r="R5" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="126"/>
-      <c r="T5" s="126"/>
-      <c r="U5" s="126"/>
-      <c r="V5" s="126"/>
-      <c r="W5" s="126"/>
-      <c r="X5" s="126"/>
-      <c r="Y5" s="126"/>
-      <c r="Z5" s="126"/>
-      <c r="AA5" s="126"/>
-      <c r="AB5" s="126"/>
-      <c r="AC5" s="126"/>
-      <c r="AD5" s="126"/>
-      <c r="AE5" s="126"/>
-      <c r="AF5" s="126"/>
-      <c r="AG5" s="126"/>
-      <c r="AH5" s="126"/>
-    </row>
-    <row r="6" spans="1:34" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="S5" s="159"/>
+      <c r="T5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
+      <c r="X5" s="159"/>
+      <c r="Y5" s="159"/>
+      <c r="Z5" s="159"/>
+      <c r="AA5" s="159"/>
+      <c r="AB5" s="159"/>
+      <c r="AC5" s="159"/>
+      <c r="AD5" s="159"/>
+      <c r="AE5" s="159"/>
+      <c r="AF5" s="159"/>
+      <c r="AG5" s="159"/>
+      <c r="AH5" s="159"/>
+    </row>
+    <row r="6" spans="1:34" s="102" customFormat="1" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="130"/>
-      <c r="B7" s="148" t="s">
+      <c r="A7" s="87"/>
+      <c r="B7" s="162" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="162" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="149" t="s">
+      <c r="D7" s="164" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="150" t="s">
+      <c r="E7" s="166" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="151" t="s">
+      <c r="F7" s="168" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="152" t="s">
+      <c r="G7" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="144"/>
-      <c r="I7" s="153" t="s">
+      <c r="H7" s="161"/>
+      <c r="I7" s="170" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="135"/>
-      <c r="L7" s="85" t="s">
+      <c r="J7" s="171"/>
+      <c r="L7" s="172" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="86" t="s">
+      <c r="M7" s="172"/>
+      <c r="N7" s="172" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="172"/>
+      <c r="P7" s="152" t="s">
         <v>42</v>
       </c>
-      <c r="R7" s="85" t="s">
+      <c r="R7" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="U7" s="85" t="s">
+      <c r="S7" s="148"/>
+      <c r="T7" s="116"/>
+      <c r="U7" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="W7" s="85" t="s">
+      <c r="V7" s="148"/>
+      <c r="W7" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="Y7" s="85" t="s">
+      <c r="X7" s="148"/>
+      <c r="Y7" s="148" t="s">
         <v>43</v>
       </c>
-      <c r="AA7" s="85" t="s">
+      <c r="Z7" s="148"/>
+      <c r="AA7" s="148" t="s">
         <v>44</v>
       </c>
-      <c r="AC7" s="85" t="s">
+      <c r="AB7" s="148"/>
+      <c r="AC7" s="148" t="s">
         <v>45</v>
       </c>
-      <c r="AE7" s="85" t="s">
+      <c r="AD7" s="148"/>
+      <c r="AE7" s="148" t="s">
         <v>46</v>
       </c>
-      <c r="AH7" s="86" t="s">
+      <c r="AF7" s="148"/>
+      <c r="AG7" s="116"/>
+      <c r="AH7" s="117" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="130"/>
-      <c r="B8" s="134"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="138"/>
-      <c r="G8" s="145" t="s">
+      <c r="A8" s="87"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="167"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="146" t="s">
+      <c r="H8" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="147" t="s">
+      <c r="I8" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="146" t="s">
+      <c r="J8" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="85" t="s">
+      <c r="L8" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="85" t="s">
+      <c r="M8" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="85" t="s">
+      <c r="N8" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="85" t="s">
+      <c r="O8" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="86"/>
-      <c r="AH8" s="86"/>
+      <c r="P8" s="153"/>
+      <c r="R8" s="113" t="s">
+        <v>9</v>
+      </c>
+      <c r="S8" s="113" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="X8" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y8" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB8" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC8" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD8" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE8" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF8" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG8" s="113"/>
+      <c r="AH8" s="114"/>
     </row>
     <row r="9" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="130"/>
-      <c r="B9" s="131" t="s">
+      <c r="A9" s="87"/>
+      <c r="B9" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="139" t="s">
+      <c r="C9" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="141">
+      <c r="D9" s="93">
         <v>38226</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="G9" s="142">
+      <c r="E9" s="90"/>
+      <c r="G9" s="94">
         <v>21.68</v>
       </c>
-      <c r="H9" s="143">
+      <c r="H9" s="95">
         <v>32.520000000000003</v>
       </c>
-      <c r="I9" s="142">
+      <c r="I9" s="94">
         <v>86639.77</v>
       </c>
-      <c r="J9" s="143">
+      <c r="J9" s="95">
         <v>138605.66</v>
       </c>
-      <c r="K9" s="85">
-        <v>0</v>
-      </c>
-      <c r="L9" s="85">
+      <c r="L9" s="100">
         <v>1837.5</v>
       </c>
-      <c r="M9" s="85">
+      <c r="M9" s="100">
         <v>12.7</v>
       </c>
-      <c r="N9" s="85">
+      <c r="N9" s="178">
         <v>87225.33</v>
       </c>
-      <c r="O9" s="85">
+      <c r="O9" s="178">
         <v>113521.61</v>
       </c>
-      <c r="P9" s="85">
+      <c r="P9" s="100">
         <v>6</v>
       </c>
+      <c r="R9" s="177">
+        <f>L9*G9</f>
+        <v>39837</v>
+      </c>
+      <c r="S9" s="177">
+        <f>M9*H9</f>
+        <v>413.00400000000002</v>
+      </c>
+      <c r="U9" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V9" s="177">
+        <f>N9*0.01 +O9*0.015</f>
+        <v>2575.0774499999998</v>
+      </c>
+      <c r="W9" s="100" t="str">
+        <f>IF(I9&lt;N9,"Oui","Non")</f>
+        <v>Oui</v>
+      </c>
+      <c r="X9" s="177" cm="1">
+        <f t="array" ref="X9">_xlfn.IFS(W9="Oui",((N9-I9)*0.1),W9="Non",0)</f>
+        <v>58.55599999999977</v>
+      </c>
+      <c r="Y9" s="100" t="str">
+        <f>IF(J9&lt;O9,"Oui","Non")</f>
+        <v>Non</v>
+      </c>
+      <c r="Z9" s="177" cm="1">
+        <f t="array" ref="Z9">_xlfn.IFS(Y9="Oui",((O9-J9)*0.15),Y9="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="100" t="str">
+        <f>IF(P9&gt;=6,"Oui","Non")</f>
+        <v>Oui</v>
+      </c>
+      <c r="AB9" s="177" cm="1">
+        <f t="array" ref="AB9">_xlfn.IFS(AA9&gt;="Oui",(N9+O9)*0.0025,AA9="Non",0)</f>
+        <v>501.86735000000004</v>
+      </c>
+      <c r="AC9" s="100" t="str">
+        <f>IF(AND(Y9="Oui",W9="Oui"),"Oui","Non")</f>
+        <v>Non</v>
+      </c>
     </row>
     <row r="10" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="130"/>
-      <c r="B10" s="131" t="s">
+      <c r="A10" s="87"/>
+      <c r="B10" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="139" t="s">
+      <c r="C10" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="141">
+      <c r="D10" s="93">
         <v>37601</v>
       </c>
-      <c r="E10" s="133"/>
-      <c r="G10" s="142">
+      <c r="E10" s="90"/>
+      <c r="G10" s="94">
         <v>23.05</v>
       </c>
-      <c r="H10" s="143">
+      <c r="H10" s="95">
         <v>34.58</v>
       </c>
-      <c r="I10" s="142">
+      <c r="I10" s="94">
         <v>86104.49</v>
       </c>
-      <c r="J10" s="143">
+      <c r="J10" s="95">
         <v>141119.44</v>
       </c>
-      <c r="K10" s="85">
-        <v>0</v>
-      </c>
-      <c r="L10" s="85">
+      <c r="L10" s="100">
         <v>1800</v>
       </c>
-      <c r="M10" s="85">
+      <c r="M10" s="100">
         <v>25.2</v>
       </c>
-      <c r="N10" s="85">
+      <c r="N10" s="178">
         <v>100494.47</v>
       </c>
-      <c r="O10" s="85">
+      <c r="O10" s="178">
         <v>133202.71</v>
       </c>
-      <c r="P10" s="85">
+      <c r="P10" s="100">
         <v>2</v>
       </c>
+      <c r="R10" s="177">
+        <f t="shared" ref="R10:R25" si="0">L10*G10</f>
+        <v>41490</v>
+      </c>
+      <c r="S10" s="177">
+        <f t="shared" ref="S10:S25" si="1">M10*H10</f>
+        <v>871.41599999999994</v>
+      </c>
+      <c r="U10" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V10" s="177">
+        <f t="shared" ref="V10:V25" si="2">N10*0.01 +O10*0.015</f>
+        <v>3002.9853499999999</v>
+      </c>
+      <c r="W10" s="100" t="str">
+        <f t="shared" ref="W10:W25" si="3">IF(I10&lt;N10,"Oui","Non")</f>
+        <v>Oui</v>
+      </c>
+      <c r="X10" s="177" cm="1">
+        <f t="array" ref="X10">_xlfn.IFS(W10="Oui",((N10-I10)*0.1),W10="Non",0)</f>
+        <v>1438.9979999999996</v>
+      </c>
+      <c r="Y10" s="100" t="str">
+        <f t="shared" ref="Y10:Y25" si="4">IF(J10&lt;O10,"Oui","Non")</f>
+        <v>Non</v>
+      </c>
+      <c r="Z10" s="177" cm="1">
+        <f t="array" ref="Z10">_xlfn.IFS(Y10="Oui",((O10-J10)*0.15),Y10="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="100" t="str">
+        <f t="shared" ref="AA10:AA25" si="5">IF(P10&gt;=6,"Oui","Non")</f>
+        <v>Non</v>
+      </c>
+      <c r="AB10" s="177" cm="1">
+        <f t="array" ref="AB10">_xlfn.IFS(AA10&gt;="Oui",(N10+O10)*0.0025,AA10="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="100" t="str">
+        <f t="shared" ref="AC10:AC25" si="6">IF(AND(Y10="Oui",W10="Oui"),"Oui","Non")</f>
+        <v>Non</v>
+      </c>
     </row>
     <row r="11" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="130"/>
-      <c r="B11" s="131" t="s">
+      <c r="A11" s="87"/>
+      <c r="B11" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="139" t="s">
+      <c r="C11" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="141">
+      <c r="D11" s="93">
         <v>35826</v>
       </c>
-      <c r="E11" s="133"/>
-      <c r="G11" s="142">
+      <c r="E11" s="90"/>
+      <c r="G11" s="94">
         <v>26.94</v>
       </c>
-      <c r="H11" s="143">
+      <c r="H11" s="95">
         <v>40.409999999999997</v>
       </c>
-      <c r="I11" s="142">
+      <c r="I11" s="94">
         <v>89605.86</v>
       </c>
-      <c r="J11" s="143">
+      <c r="J11" s="95">
         <v>156292.04</v>
       </c>
-      <c r="K11" s="85">
-        <v>0</v>
-      </c>
-      <c r="L11" s="85">
+      <c r="L11" s="100">
         <v>1800</v>
       </c>
-      <c r="M11" s="85">
-        <v>0</v>
-      </c>
-      <c r="N11" s="85">
+      <c r="M11" s="100">
+        <v>0</v>
+      </c>
+      <c r="N11" s="178">
         <v>76821.77</v>
       </c>
-      <c r="O11" s="85">
+      <c r="O11" s="178">
         <v>158727.13</v>
       </c>
-      <c r="P11" s="85">
+      <c r="P11" s="100">
         <v>6</v>
       </c>
+      <c r="R11" s="177">
+        <f t="shared" si="0"/>
+        <v>48492</v>
+      </c>
+      <c r="S11" s="177">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V11" s="177">
+        <f t="shared" si="2"/>
+        <v>3149.1246500000002</v>
+      </c>
+      <c r="W11" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X11" s="177" cm="1">
+        <f t="array" ref="X11">_xlfn.IFS(W11="Oui",((N11-I11)*0.1),W11="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z11" s="177" cm="1">
+        <f t="array" ref="Z11">_xlfn.IFS(Y11="Oui",((O11-J11)*0.15),Y11="Non",0)</f>
+        <v>365.26349999999945</v>
+      </c>
+      <c r="AA11" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB11" s="177" cm="1">
+        <f t="array" ref="AB11">_xlfn.IFS(AA11&gt;="Oui",(N11+O11)*0.0025,AA11="Non",0)</f>
+        <v>588.87225000000012</v>
+      </c>
+      <c r="AC11" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
     </row>
     <row r="12" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="130"/>
-      <c r="B12" s="131" t="s">
+      <c r="A12" s="87"/>
+      <c r="B12" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="139" t="s">
+      <c r="C12" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="141">
+      <c r="D12" s="93">
         <v>35403</v>
       </c>
-      <c r="E12" s="133"/>
-      <c r="G12" s="142">
+      <c r="E12" s="90"/>
+      <c r="G12" s="94">
         <v>27.87</v>
       </c>
-      <c r="H12" s="143">
+      <c r="H12" s="95">
         <v>41.81</v>
       </c>
-      <c r="I12" s="142">
+      <c r="I12" s="94">
         <v>88556.09</v>
       </c>
-      <c r="J12" s="143">
+      <c r="J12" s="95">
         <v>156576.41</v>
       </c>
-      <c r="K12" s="85">
-        <v>0</v>
-      </c>
-      <c r="L12" s="85">
+      <c r="L12" s="100">
         <v>1762.5</v>
       </c>
-      <c r="M12" s="85">
-        <v>0</v>
-      </c>
-      <c r="N12" s="85">
+      <c r="M12" s="100">
+        <v>0</v>
+      </c>
+      <c r="N12" s="178">
         <v>77813.539999999994</v>
       </c>
-      <c r="O12" s="85">
+      <c r="O12" s="178">
         <v>170576.59</v>
       </c>
-      <c r="P12" s="85">
+      <c r="P12" s="100">
         <v>9</v>
       </c>
+      <c r="R12" s="177">
+        <f t="shared" si="0"/>
+        <v>49120.875</v>
+      </c>
+      <c r="S12" s="177">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U12" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V12" s="177">
+        <f t="shared" si="2"/>
+        <v>3336.7842500000002</v>
+      </c>
+      <c r="W12" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X12" s="177" cm="1">
+        <f t="array" ref="X12">_xlfn.IFS(W12="Oui",((N12-I12)*0.1),W12="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z12" s="177" cm="1">
+        <f t="array" ref="Z12">_xlfn.IFS(Y12="Oui",((O12-J12)*0.15),Y12="Non",0)</f>
+        <v>2100.0269999999987</v>
+      </c>
+      <c r="AA12" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB12" s="177" cm="1">
+        <f t="array" ref="AB12">_xlfn.IFS(AA12&gt;="Oui",(N12+O12)*0.0025,AA12="Non",0)</f>
+        <v>620.975325</v>
+      </c>
+      <c r="AC12" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
     </row>
     <row r="13" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="130"/>
-      <c r="B13" s="131" t="s">
+      <c r="A13" s="87"/>
+      <c r="B13" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="139" t="s">
+      <c r="C13" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="141">
+      <c r="D13" s="93">
         <v>33093</v>
       </c>
-      <c r="E13" s="133"/>
-      <c r="G13" s="142">
+      <c r="E13" s="90"/>
+      <c r="G13" s="94">
         <v>32.93</v>
       </c>
-      <c r="H13" s="143">
+      <c r="H13" s="95">
         <v>49.4</v>
       </c>
-      <c r="I13" s="142">
+      <c r="I13" s="94">
         <v>91038.77</v>
       </c>
-      <c r="J13" s="143">
+      <c r="J13" s="95">
         <v>172168.01</v>
       </c>
-      <c r="K13" s="85">
-        <v>0</v>
-      </c>
-      <c r="L13" s="85">
+      <c r="L13" s="100">
         <v>1725</v>
       </c>
-      <c r="M13" s="85">
+      <c r="M13" s="100">
         <v>39.57</v>
       </c>
-      <c r="N13" s="85">
+      <c r="N13" s="178">
         <v>96236.12</v>
       </c>
-      <c r="O13" s="85">
+      <c r="O13" s="178">
         <v>177509.88</v>
       </c>
-      <c r="P13" s="85">
+      <c r="P13" s="100">
         <v>7</v>
       </c>
+      <c r="R13" s="177">
+        <f t="shared" si="0"/>
+        <v>56804.25</v>
+      </c>
+      <c r="S13" s="177">
+        <f t="shared" si="1"/>
+        <v>1954.758</v>
+      </c>
+      <c r="U13" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V13" s="177">
+        <f t="shared" si="2"/>
+        <v>3625.0093999999999</v>
+      </c>
+      <c r="W13" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Oui</v>
+      </c>
+      <c r="X13" s="177" cm="1">
+        <f t="array" ref="X13">_xlfn.IFS(W13="Oui",((N13-I13)*0.1),W13="Non",0)</f>
+        <v>519.7349999999991</v>
+      </c>
+      <c r="Y13" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z13" s="177" cm="1">
+        <f t="array" ref="Z13">_xlfn.IFS(Y13="Oui",((O13-J13)*0.15),Y13="Non",0)</f>
+        <v>801.28049999999928</v>
+      </c>
+      <c r="AA13" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB13" s="177" cm="1">
+        <f t="array" ref="AB13">_xlfn.IFS(AA13&gt;="Oui",(N13+O13)*0.0025,AA13="Non",0)</f>
+        <v>684.36500000000001</v>
+      </c>
+      <c r="AC13" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
     </row>
     <row r="14" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="130"/>
-      <c r="B14" s="131" t="s">
+      <c r="A14" s="87"/>
+      <c r="B14" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="139" t="s">
+      <c r="C14" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="141">
+      <c r="D14" s="93">
         <v>37900</v>
       </c>
-      <c r="E14" s="133"/>
-      <c r="G14" s="142">
+      <c r="E14" s="90"/>
+      <c r="G14" s="94">
         <v>22.4</v>
       </c>
-      <c r="H14" s="143">
+      <c r="H14" s="95">
         <v>33.6</v>
       </c>
-      <c r="I14" s="142">
+      <c r="I14" s="94">
         <v>87296.23</v>
       </c>
-      <c r="J14" s="143">
+      <c r="J14" s="95">
         <v>141450.34</v>
       </c>
-      <c r="K14" s="85">
-        <v>0</v>
-      </c>
-      <c r="L14" s="85">
+      <c r="L14" s="100">
         <v>1837.5</v>
       </c>
-      <c r="M14" s="85">
+      <c r="M14" s="100">
         <v>98.2</v>
       </c>
-      <c r="N14" s="85">
+      <c r="N14" s="178">
         <v>86363.33</v>
       </c>
-      <c r="O14" s="85">
+      <c r="O14" s="178">
         <v>120584.13</v>
       </c>
-      <c r="P14" s="85">
+      <c r="P14" s="100">
         <v>6</v>
       </c>
+      <c r="R14" s="177">
+        <f t="shared" si="0"/>
+        <v>41160</v>
+      </c>
+      <c r="S14" s="177">
+        <f t="shared" si="1"/>
+        <v>3299.5200000000004</v>
+      </c>
+      <c r="U14" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V14" s="177">
+        <f t="shared" si="2"/>
+        <v>2672.39525</v>
+      </c>
+      <c r="W14" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X14" s="177" cm="1">
+        <f t="array" ref="X14">_xlfn.IFS(W14="Oui",((N14-I14)*0.1),W14="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Non</v>
+      </c>
+      <c r="Z14" s="177" cm="1">
+        <f t="array" ref="Z14">_xlfn.IFS(Y14="Oui",((O14-J14)*0.15),Y14="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB14" s="177" cm="1">
+        <f t="array" ref="AB14">_xlfn.IFS(AA14&gt;="Oui",(N14+O14)*0.0025,AA14="Non",0)</f>
+        <v>517.36865000000012</v>
+      </c>
+      <c r="AC14" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
     </row>
     <row r="15" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="130"/>
-      <c r="B15" s="131" t="s">
+      <c r="A15" s="87"/>
+      <c r="B15" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="139" t="s">
+      <c r="C15" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="141">
+      <c r="D15" s="93">
         <v>35590</v>
       </c>
-      <c r="E15" s="133"/>
-      <c r="G15" s="142">
+      <c r="E15" s="90"/>
+      <c r="G15" s="94">
         <v>27.46</v>
       </c>
-      <c r="H15" s="143">
+      <c r="H15" s="95">
         <v>41.19</v>
       </c>
-      <c r="I15" s="142">
+      <c r="I15" s="94">
         <v>88194.9</v>
       </c>
-      <c r="J15" s="143">
+      <c r="J15" s="95">
         <v>155011.24</v>
       </c>
-      <c r="K15" s="85">
-        <v>0</v>
-      </c>
-      <c r="L15" s="85">
+      <c r="L15" s="100">
         <v>1762.5</v>
       </c>
-      <c r="M15" s="85">
+      <c r="M15" s="100">
         <v>244.14</v>
       </c>
-      <c r="N15" s="85">
+      <c r="N15" s="178">
         <v>98812.43</v>
       </c>
-      <c r="O15" s="85">
+      <c r="O15" s="178">
         <v>119521.7</v>
       </c>
-      <c r="P15" s="85">
+      <c r="P15" s="100">
         <v>6</v>
       </c>
+      <c r="R15" s="177">
+        <f t="shared" si="0"/>
+        <v>48398.25</v>
+      </c>
+      <c r="S15" s="177">
+        <f t="shared" si="1"/>
+        <v>10056.1266</v>
+      </c>
+      <c r="U15" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V15" s="177">
+        <f t="shared" si="2"/>
+        <v>2780.9497999999999</v>
+      </c>
+      <c r="W15" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Oui</v>
+      </c>
+      <c r="X15" s="177" cm="1">
+        <f t="array" ref="X15">_xlfn.IFS(W15="Oui",((N15-I15)*0.1),W15="Non",0)</f>
+        <v>1061.7529999999999</v>
+      </c>
+      <c r="Y15" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Non</v>
+      </c>
+      <c r="Z15" s="177" cm="1">
+        <f t="array" ref="Z15">_xlfn.IFS(Y15="Oui",((O15-J15)*0.15),Y15="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB15" s="177" cm="1">
+        <f t="array" ref="AB15">_xlfn.IFS(AA15&gt;="Oui",(N15+O15)*0.0025,AA15="Non",0)</f>
+        <v>545.83532500000001</v>
+      </c>
+      <c r="AC15" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
     </row>
     <row r="16" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="130"/>
-      <c r="B16" s="131" t="s">
+      <c r="A16" s="87"/>
+      <c r="B16" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="139" t="s">
+      <c r="C16" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="141">
+      <c r="D16" s="93">
         <v>35192</v>
       </c>
-      <c r="E16" s="133"/>
-      <c r="G16" s="142">
+      <c r="E16" s="90"/>
+      <c r="G16" s="94">
         <v>28.33</v>
       </c>
-      <c r="H16" s="143">
+      <c r="H16" s="95">
         <v>42.5</v>
       </c>
-      <c r="I16" s="142">
+      <c r="I16" s="94">
         <v>88963.64</v>
       </c>
-      <c r="J16" s="143">
+      <c r="J16" s="95">
         <v>158342.45000000001</v>
       </c>
-      <c r="K16" s="85">
-        <v>0</v>
-      </c>
-      <c r="L16" s="85">
+      <c r="L16" s="100">
         <v>1762.5</v>
       </c>
-      <c r="M16" s="85">
+      <c r="M16" s="100">
         <v>109.39</v>
       </c>
-      <c r="N16" s="85">
+      <c r="N16" s="178">
         <v>89879.18</v>
       </c>
-      <c r="O16" s="85">
+      <c r="O16" s="178">
         <v>164850.17000000001</v>
       </c>
-      <c r="P16" s="85">
+      <c r="P16" s="100">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="130"/>
-      <c r="B17" s="131" t="s">
+      <c r="R16" s="177">
+        <f t="shared" si="0"/>
+        <v>49931.625</v>
+      </c>
+      <c r="S16" s="177">
+        <f t="shared" si="1"/>
+        <v>4649.0749999999998</v>
+      </c>
+      <c r="U16" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V16" s="177">
+        <f t="shared" si="2"/>
+        <v>3371.5443500000001</v>
+      </c>
+      <c r="W16" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Oui</v>
+      </c>
+      <c r="X16" s="177" cm="1">
+        <f t="array" ref="X16">_xlfn.IFS(W16="Oui",((N16-I16)*0.1),W16="Non",0)</f>
+        <v>91.553999999999363</v>
+      </c>
+      <c r="Y16" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z16" s="177" cm="1">
+        <f t="array" ref="Z16">_xlfn.IFS(Y16="Oui",((O16-J16)*0.15),Y16="Non",0)</f>
+        <v>976.15800000000013</v>
+      </c>
+      <c r="AA16" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="AB16" s="177" cm="1">
+        <f t="array" ref="AB16">_xlfn.IFS(AA16&gt;="Oui",(N16+O16)*0.0025,AA16="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="87"/>
+      <c r="B17" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="139" t="s">
+      <c r="C17" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="141">
+      <c r="D17" s="93">
         <v>36628</v>
       </c>
-      <c r="E17" s="133"/>
-      <c r="G17" s="142">
+      <c r="E17" s="90"/>
+      <c r="G17" s="94">
         <v>25.19</v>
       </c>
-      <c r="H17" s="143">
+      <c r="H17" s="95">
         <v>37.78</v>
       </c>
-      <c r="I17" s="142">
+      <c r="I17" s="94">
         <v>88023.83</v>
       </c>
-      <c r="J17" s="143">
+      <c r="J17" s="95">
         <v>149436.59</v>
       </c>
-      <c r="K17" s="85">
-        <v>0</v>
-      </c>
-      <c r="L17" s="85">
+      <c r="L17" s="100">
         <v>1800</v>
       </c>
-      <c r="M17" s="85">
-        <v>0</v>
-      </c>
-      <c r="N17" s="85">
+      <c r="M17" s="100">
+        <v>0</v>
+      </c>
+      <c r="N17" s="178">
         <v>92616.29</v>
       </c>
-      <c r="O17" s="85">
+      <c r="O17" s="178">
         <v>149766.94</v>
       </c>
-      <c r="P17" s="85">
+      <c r="P17" s="100">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="130"/>
-      <c r="B18" s="131" t="s">
+      <c r="R17" s="177">
+        <f t="shared" si="0"/>
+        <v>45342</v>
+      </c>
+      <c r="S17" s="177">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V17" s="177">
+        <f t="shared" si="2"/>
+        <v>3172.6669999999999</v>
+      </c>
+      <c r="W17" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Oui</v>
+      </c>
+      <c r="X17" s="177" cm="1">
+        <f t="array" ref="X17">_xlfn.IFS(W17="Oui",((N17-I17)*0.1),W17="Non",0)</f>
+        <v>459.24599999999919</v>
+      </c>
+      <c r="Y17" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z17" s="177" cm="1">
+        <f t="array" ref="Z17">_xlfn.IFS(Y17="Oui",((O17-J17)*0.15),Y17="Non",0)</f>
+        <v>49.552500000000869</v>
+      </c>
+      <c r="AA17" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB17" s="177" cm="1">
+        <f t="array" ref="AB17">_xlfn.IFS(AA17&gt;="Oui",(N17+O17)*0.0025,AA17="Non",0)</f>
+        <v>605.95807500000001</v>
+      </c>
+      <c r="AC17" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="87"/>
+      <c r="B18" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="139" t="s">
+      <c r="C18" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="141">
+      <c r="D18" s="93">
         <v>30115</v>
       </c>
-      <c r="E18" s="133"/>
-      <c r="G18" s="142">
+      <c r="E18" s="90"/>
+      <c r="G18" s="94">
         <v>39.46</v>
       </c>
-      <c r="H18" s="143">
+      <c r="H18" s="95">
         <v>59.19</v>
       </c>
-      <c r="I18" s="142">
+      <c r="I18" s="94">
         <v>92465.44</v>
       </c>
-      <c r="J18" s="143">
+      <c r="J18" s="95">
         <v>188016.91</v>
       </c>
-      <c r="K18" s="85">
-        <v>0</v>
-      </c>
-      <c r="L18" s="85">
+      <c r="L18" s="100">
         <v>1650</v>
       </c>
-      <c r="M18" s="85">
+      <c r="M18" s="100">
         <v>143.27000000000001</v>
       </c>
-      <c r="N18" s="85">
+      <c r="N18" s="178">
         <v>86538.68</v>
       </c>
-      <c r="O18" s="85">
+      <c r="O18" s="178">
         <v>168507.1</v>
       </c>
-      <c r="P18" s="85">
+      <c r="P18" s="100">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="130"/>
-      <c r="B19" s="131" t="s">
+      <c r="R18" s="177">
+        <f t="shared" si="0"/>
+        <v>65109</v>
+      </c>
+      <c r="S18" s="177">
+        <f t="shared" si="1"/>
+        <v>8480.1512999999995</v>
+      </c>
+      <c r="U18" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V18" s="177">
+        <f t="shared" si="2"/>
+        <v>3392.9933000000001</v>
+      </c>
+      <c r="W18" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X18" s="177" cm="1">
+        <f t="array" ref="X18">_xlfn.IFS(W18="Oui",((N18-I18)*0.1),W18="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Non</v>
+      </c>
+      <c r="Z18" s="177" cm="1">
+        <f t="array" ref="Z18">_xlfn.IFS(Y18="Oui",((O18-J18)*0.15),Y18="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="AB18" s="177" cm="1">
+        <f t="array" ref="AB18">_xlfn.IFS(AA18&gt;="Oui",(N18+O18)*0.0025,AA18="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC18" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="87"/>
+      <c r="B19" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="139" t="s">
+      <c r="C19" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="141">
+      <c r="D19" s="93">
         <v>41231</v>
       </c>
-      <c r="E19" s="133"/>
-      <c r="G19" s="142">
+      <c r="E19" s="90"/>
+      <c r="G19" s="94">
         <v>15.1</v>
       </c>
-      <c r="H19" s="143">
+      <c r="H19" s="95">
         <v>22.64</v>
       </c>
-      <c r="I19" s="142">
+      <c r="I19" s="94">
         <v>82233.27</v>
       </c>
-      <c r="J19" s="143">
+      <c r="J19" s="95">
         <v>114677.5</v>
       </c>
-      <c r="K19" s="85">
-        <v>0</v>
-      </c>
-      <c r="L19" s="85">
+      <c r="L19" s="100">
         <v>1875</v>
       </c>
-      <c r="M19" s="85">
-        <v>0</v>
-      </c>
-      <c r="N19" s="85">
+      <c r="M19" s="100">
+        <v>0</v>
+      </c>
+      <c r="N19" s="178">
         <v>74240.86</v>
       </c>
-      <c r="O19" s="85">
+      <c r="O19" s="178">
         <v>112740.09</v>
       </c>
-      <c r="P19" s="85">
+      <c r="P19" s="100">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="130"/>
-      <c r="B20" s="131" t="s">
+      <c r="R19" s="177">
+        <f t="shared" si="0"/>
+        <v>28312.5</v>
+      </c>
+      <c r="S19" s="177">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V19" s="177">
+        <f t="shared" si="2"/>
+        <v>2433.5099499999997</v>
+      </c>
+      <c r="W19" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X19" s="177" cm="1">
+        <f t="array" ref="X19">_xlfn.IFS(W19="Oui",((N19-I19)*0.1),W19="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Non</v>
+      </c>
+      <c r="Z19" s="177" cm="1">
+        <f t="array" ref="Z19">_xlfn.IFS(Y19="Oui",((O19-J19)*0.15),Y19="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="AB19" s="177" cm="1">
+        <f t="array" ref="AB19">_xlfn.IFS(AA19&gt;="Oui",(N19+O19)*0.0025,AA19="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="87"/>
+      <c r="B20" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="139" t="s">
+      <c r="C20" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="141">
+      <c r="D20" s="93">
         <v>31824</v>
       </c>
-      <c r="E20" s="133"/>
-      <c r="G20" s="142">
+      <c r="E20" s="90"/>
+      <c r="G20" s="94">
         <v>35.71</v>
       </c>
-      <c r="H20" s="143">
+      <c r="H20" s="95">
         <v>53.57</v>
       </c>
-      <c r="I20" s="142">
+      <c r="I20" s="94">
         <v>91406.45</v>
       </c>
-      <c r="J20" s="143">
+      <c r="J20" s="95">
         <v>178594.61</v>
       </c>
-      <c r="K20" s="85">
-        <v>0</v>
-      </c>
-      <c r="L20" s="85">
+      <c r="L20" s="100">
         <v>1687.5</v>
       </c>
-      <c r="M20" s="85">
+      <c r="M20" s="100">
         <v>145.13</v>
       </c>
-      <c r="N20" s="85">
+      <c r="N20" s="178">
         <v>90744.11</v>
       </c>
-      <c r="O20" s="85">
+      <c r="O20" s="178">
         <v>180217.79</v>
       </c>
-      <c r="P20" s="85">
+      <c r="P20" s="100">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="130"/>
-      <c r="B21" s="131" t="s">
+      <c r="R20" s="177">
+        <f t="shared" si="0"/>
+        <v>60260.625</v>
+      </c>
+      <c r="S20" s="177">
+        <f t="shared" si="1"/>
+        <v>7774.6140999999998</v>
+      </c>
+      <c r="U20" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V20" s="177">
+        <f t="shared" si="2"/>
+        <v>3610.70795</v>
+      </c>
+      <c r="W20" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X20" s="177" cm="1">
+        <f t="array" ref="X20">_xlfn.IFS(W20="Oui",((N20-I20)*0.1),W20="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z20" s="177" cm="1">
+        <f t="array" ref="Z20">_xlfn.IFS(Y20="Oui",((O20-J20)*0.15),Y20="Non",0)</f>
+        <v>243.4770000000033</v>
+      </c>
+      <c r="AA20" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB20" s="177" cm="1">
+        <f t="array" ref="AB20">_xlfn.IFS(AA20&gt;="Oui",(N20+O20)*0.0025,AA20="Non",0)</f>
+        <v>677.40475000000004</v>
+      </c>
+      <c r="AC20" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="87"/>
+      <c r="B21" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="139" t="s">
+      <c r="C21" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="141">
+      <c r="D21" s="93">
         <v>38150</v>
       </c>
-      <c r="E21" s="133"/>
-      <c r="G21" s="142">
+      <c r="E21" s="90"/>
+      <c r="G21" s="94">
         <v>21.85</v>
       </c>
-      <c r="H21" s="143">
+      <c r="H21" s="95">
         <v>32.770000000000003</v>
       </c>
-      <c r="I21" s="142">
+      <c r="I21" s="94">
         <v>86792.81</v>
       </c>
-      <c r="J21" s="143">
+      <c r="J21" s="95">
         <v>139268.84</v>
       </c>
-      <c r="K21" s="85">
-        <v>0</v>
-      </c>
-      <c r="L21" s="85">
+      <c r="L21" s="100">
         <v>1837.5</v>
       </c>
-      <c r="M21" s="85">
+      <c r="M21" s="100">
         <v>191.85</v>
       </c>
-      <c r="N21" s="85">
+      <c r="N21" s="178">
         <v>92277.83</v>
       </c>
-      <c r="O21" s="85">
+      <c r="O21" s="178">
         <v>139124.15</v>
       </c>
-      <c r="P21" s="85">
+      <c r="P21" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="130"/>
-      <c r="B22" s="131" t="s">
+      <c r="R21" s="177">
+        <f t="shared" si="0"/>
+        <v>40149.375</v>
+      </c>
+      <c r="S21" s="177">
+        <f t="shared" si="1"/>
+        <v>6286.9245000000001</v>
+      </c>
+      <c r="U21" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V21" s="177">
+        <f t="shared" si="2"/>
+        <v>3009.6405499999996</v>
+      </c>
+      <c r="W21" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Oui</v>
+      </c>
+      <c r="X21" s="177" cm="1">
+        <f t="array" ref="X21">_xlfn.IFS(W21="Oui",((N21-I21)*0.1),W21="Non",0)</f>
+        <v>548.50200000000041</v>
+      </c>
+      <c r="Y21" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Non</v>
+      </c>
+      <c r="Z21" s="177" cm="1">
+        <f t="array" ref="Z21">_xlfn.IFS(Y21="Oui",((O21-J21)*0.15),Y21="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="AB21" s="177" cm="1">
+        <f t="array" ref="AB21">_xlfn.IFS(AA21&gt;="Oui",(N21+O21)*0.0025,AA21="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="87"/>
+      <c r="B22" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="139" t="s">
+      <c r="C22" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="141">
+      <c r="D22" s="93">
         <v>32891</v>
       </c>
-      <c r="E22" s="133"/>
-      <c r="G22" s="142">
+      <c r="E22" s="90"/>
+      <c r="G22" s="94">
         <v>33.380000000000003</v>
       </c>
-      <c r="H22" s="143">
+      <c r="H22" s="95">
         <v>50.06</v>
       </c>
-      <c r="I22" s="142">
+      <c r="I22" s="94">
         <v>91420.63</v>
       </c>
-      <c r="J22" s="143">
+      <c r="J22" s="95">
         <v>173822.75</v>
       </c>
-      <c r="K22" s="85">
-        <v>0</v>
-      </c>
-      <c r="L22" s="85">
+      <c r="L22" s="100">
         <v>1725</v>
       </c>
-      <c r="M22" s="85">
+      <c r="M22" s="100">
         <v>150.72</v>
       </c>
-      <c r="N22" s="85">
+      <c r="N22" s="178">
         <v>80527.14</v>
       </c>
-      <c r="O22" s="85">
+      <c r="O22" s="178">
         <v>181545.58</v>
       </c>
-      <c r="P22" s="85">
+      <c r="P22" s="100">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="130"/>
-      <c r="B23" s="131" t="s">
+      <c r="R22" s="177">
+        <f t="shared" si="0"/>
+        <v>57580.500000000007</v>
+      </c>
+      <c r="S22" s="177">
+        <f t="shared" si="1"/>
+        <v>7545.0432000000001</v>
+      </c>
+      <c r="U22" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V22" s="177">
+        <f t="shared" si="2"/>
+        <v>3528.4550999999997</v>
+      </c>
+      <c r="W22" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X22" s="177" cm="1">
+        <f t="array" ref="X22">_xlfn.IFS(W22="Oui",((N22-I22)*0.1),W22="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z22" s="177" cm="1">
+        <f t="array" ref="Z22">_xlfn.IFS(Y22="Oui",((O22-J22)*0.15),Y22="Non",0)</f>
+        <v>1158.424499999998</v>
+      </c>
+      <c r="AA22" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="AB22" s="177" cm="1">
+        <f t="array" ref="AB22">_xlfn.IFS(AA22&gt;="Oui",(N22+O22)*0.0025,AA22="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="87"/>
+      <c r="B23" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="139" t="s">
+      <c r="C23" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="141">
+      <c r="D23" s="93">
         <v>41102</v>
       </c>
-      <c r="E23" s="133"/>
-      <c r="G23" s="142">
+      <c r="E23" s="90"/>
+      <c r="G23" s="94">
         <v>15.38</v>
       </c>
-      <c r="H23" s="143">
+      <c r="H23" s="95">
         <v>23.07</v>
       </c>
-      <c r="I23" s="142">
+      <c r="I23" s="94">
         <v>82498.34</v>
       </c>
-      <c r="J23" s="143">
+      <c r="J23" s="95">
         <v>115826.13</v>
       </c>
-      <c r="K23" s="85">
-        <v>0</v>
-      </c>
-      <c r="L23" s="85">
+      <c r="L23" s="100">
         <v>1875</v>
       </c>
-      <c r="M23" s="85">
+      <c r="M23" s="100">
         <v>159.16999999999999</v>
       </c>
-      <c r="N23" s="85">
+      <c r="N23" s="178">
         <v>73878.58</v>
       </c>
-      <c r="O23" s="85">
+      <c r="O23" s="178">
         <v>125469.62</v>
       </c>
-      <c r="P23" s="85">
+      <c r="P23" s="100">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="130"/>
-      <c r="B24" s="132" t="s">
+      <c r="R23" s="177">
+        <f t="shared" si="0"/>
+        <v>28837.5</v>
+      </c>
+      <c r="S23" s="177">
+        <f t="shared" si="1"/>
+        <v>3672.0518999999999</v>
+      </c>
+      <c r="U23" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V23" s="177">
+        <f t="shared" si="2"/>
+        <v>2620.8300999999997</v>
+      </c>
+      <c r="W23" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X23" s="177" cm="1">
+        <f t="array" ref="X23">_xlfn.IFS(W23="Oui",((N23-I23)*0.1),W23="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z23" s="177" cm="1">
+        <f t="array" ref="Z23">_xlfn.IFS(Y23="Oui",((O23-J23)*0.15),Y23="Non",0)</f>
+        <v>1446.5234999999986</v>
+      </c>
+      <c r="AA23" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB23" s="177" cm="1">
+        <f t="array" ref="AB23">_xlfn.IFS(AA23&gt;="Oui",(N23+O23)*0.0025,AA23="Non",0)</f>
+        <v>498.37050000000005</v>
+      </c>
+      <c r="AC23" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="87"/>
+      <c r="B24" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="140" t="s">
+      <c r="C24" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="141">
+      <c r="D24" s="93">
         <v>29465</v>
       </c>
-      <c r="E24" s="133"/>
-      <c r="G24" s="142">
+      <c r="E24" s="90"/>
+      <c r="G24" s="94">
         <v>40.880000000000003</v>
       </c>
-      <c r="H24" s="143">
+      <c r="H24" s="95">
         <v>61.33</v>
       </c>
-      <c r="I24" s="142">
+      <c r="I24" s="94">
         <v>93640.78</v>
       </c>
-      <c r="J24" s="143">
+      <c r="J24" s="95">
         <v>193110.06</v>
       </c>
-      <c r="K24" s="85">
-        <v>0</v>
-      </c>
-      <c r="L24" s="85">
+      <c r="L24" s="100">
         <v>1650</v>
       </c>
-      <c r="M24" s="85">
-        <v>0</v>
-      </c>
-      <c r="N24" s="85">
+      <c r="M24" s="100">
+        <v>0</v>
+      </c>
+      <c r="N24" s="178">
         <v>83732.44</v>
       </c>
-      <c r="O24" s="85">
+      <c r="O24" s="178">
         <v>208951.82</v>
       </c>
-      <c r="P24" s="85">
+      <c r="P24" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="130"/>
-      <c r="B25" s="132" t="s">
+      <c r="R24" s="177">
+        <f t="shared" si="0"/>
+        <v>67452</v>
+      </c>
+      <c r="S24" s="177">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V24" s="177">
+        <f t="shared" si="2"/>
+        <v>3971.6017000000002</v>
+      </c>
+      <c r="W24" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Non</v>
+      </c>
+      <c r="X24" s="177" cm="1">
+        <f t="array" ref="X24">_xlfn.IFS(W24="Oui",((N24-I24)*0.1),W24="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z24" s="177" cm="1">
+        <f t="array" ref="Z24">_xlfn.IFS(Y24="Oui",((O24-J24)*0.15),Y24="Non",0)</f>
+        <v>2376.2640000000015</v>
+      </c>
+      <c r="AA24" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="AB24" s="177" cm="1">
+        <f t="array" ref="AB24">_xlfn.IFS(AA24&gt;="Oui",(N24+O24)*0.0025,AA24="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="87"/>
+      <c r="B25" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="140" t="s">
+      <c r="C25" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="141">
+      <c r="D25" s="93">
         <v>30711</v>
       </c>
-      <c r="E25" s="133"/>
-      <c r="G25" s="142">
+      <c r="E25" s="90"/>
+      <c r="G25" s="94">
         <v>38.15</v>
       </c>
-      <c r="H25" s="143">
+      <c r="H25" s="95">
         <v>57.23</v>
       </c>
-      <c r="I25" s="142">
+      <c r="I25" s="94">
         <v>93464.74</v>
       </c>
-      <c r="J25" s="143">
+      <c r="J25" s="95">
         <v>187513.86</v>
       </c>
-      <c r="K25" s="85">
-        <v>0</v>
-      </c>
-      <c r="L25" s="85">
+      <c r="L25" s="100">
         <v>1687.5</v>
       </c>
-      <c r="M25" s="85">
+      <c r="M25" s="100">
         <v>226.41</v>
       </c>
-      <c r="N25" s="85">
+      <c r="N25" s="178">
         <v>98278.63</v>
       </c>
-      <c r="O25" s="85">
+      <c r="O25" s="178">
         <v>171337.91</v>
       </c>
-      <c r="P25" s="85">
+      <c r="P25" s="100">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B29" s="85" t="s">
+      <c r="R25" s="177">
+        <f t="shared" si="0"/>
+        <v>64378.125</v>
+      </c>
+      <c r="S25" s="177">
+        <f t="shared" si="1"/>
+        <v>12957.444299999999</v>
+      </c>
+      <c r="U25" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="V25" s="177">
+        <f t="shared" si="2"/>
+        <v>3552.8549500000004</v>
+      </c>
+      <c r="W25" s="100" t="str">
+        <f t="shared" si="3"/>
+        <v>Oui</v>
+      </c>
+      <c r="X25" s="177" cm="1">
+        <f t="array" ref="X25">_xlfn.IFS(W25="Oui",((N25-I25)*0.1),W25="Non",0)</f>
+        <v>481.38899999999995</v>
+      </c>
+      <c r="Y25" s="100" t="str">
+        <f t="shared" si="4"/>
+        <v>Non</v>
+      </c>
+      <c r="Z25" s="177" cm="1">
+        <f t="array" ref="Z25">_xlfn.IFS(Y25="Oui",((O25-J25)*0.1),Y25="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="100" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="AB25" s="177" cm="1">
+        <f t="array" ref="AB25">_xlfn.IFS(AA25&gt;="Oui",(N25+O25)*0.0025,AA25="Non",0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC25" s="100" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" ht="4.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I26" s="101"/>
+      <c r="J26" s="101"/>
+      <c r="N26" s="178"/>
+      <c r="O26" s="178"/>
+      <c r="V26" s="118"/>
+      <c r="X26" s="118"/>
+      <c r="AB26" s="177"/>
+    </row>
+    <row r="27" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I27" s="179">
+        <f>SUM(I10:I26)</f>
+        <v>1421706.2700000003</v>
+      </c>
+      <c r="J27" s="180">
+        <f>SUM(J10:J26)</f>
+        <v>2521227.1800000002</v>
+      </c>
+      <c r="M27" s="109"/>
+      <c r="N27" s="178">
+        <f>SUM(N9:N25)</f>
+        <v>1486480.73</v>
+      </c>
+      <c r="O27" s="178">
+        <f>SUM(O9:O25)</f>
+        <v>2596154.92</v>
+      </c>
+      <c r="P27" s="108"/>
+      <c r="R27" s="181">
+        <f>SUM(R9:R25)</f>
+        <v>832655.625</v>
+      </c>
+      <c r="S27" s="182">
+        <f>SUM(S9:S25)</f>
+        <v>67960.128899999996</v>
+      </c>
+      <c r="V27" s="183">
+        <f>SUM(V9:V25)</f>
+        <v>53807.131099999991</v>
+      </c>
+      <c r="X27" s="183">
+        <f>SUM(X9:X25)</f>
+        <v>4659.7329999999974</v>
+      </c>
+      <c r="Y27" s="108"/>
+      <c r="Z27" s="183">
+        <f>SUM(Z9:Z25)</f>
+        <v>9516.9704999999994</v>
+      </c>
+      <c r="AA27" s="111"/>
+      <c r="AB27" s="177">
+        <f>SUM(AB9:AB25)</f>
+        <v>5241.0172250000005</v>
+      </c>
+      <c r="AC27" s="108"/>
+      <c r="AD27" s="112"/>
+      <c r="AE27" s="108"/>
+      <c r="AF27" s="112"/>
+      <c r="AG27" s="110"/>
+      <c r="AH27" s="110"/>
+      <c r="AI27" s="108"/>
+    </row>
+    <row r="28" spans="1:35" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B29" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="85" t="s">
+      <c r="C29" s="150"/>
+      <c r="D29" s="150"/>
+      <c r="E29" s="149" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="85" t="s">
+      <c r="F29" s="151"/>
+      <c r="G29" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="R29" s="85" t="s">
+      <c r="H29" s="150"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="150"/>
+      <c r="L29" s="150"/>
+      <c r="M29" s="150"/>
+      <c r="N29" s="150"/>
+      <c r="O29" s="150"/>
+      <c r="P29" s="151"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="149" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="S29" s="150"/>
+      <c r="T29" s="150"/>
+      <c r="U29" s="150"/>
+      <c r="V29" s="150"/>
+      <c r="W29" s="150"/>
+      <c r="X29" s="150"/>
+      <c r="Y29" s="150"/>
+      <c r="Z29" s="150"/>
+      <c r="AA29" s="150"/>
+      <c r="AB29" s="150"/>
+      <c r="AC29" s="150"/>
+      <c r="AD29" s="150"/>
+      <c r="AE29" s="150"/>
+      <c r="AF29" s="150"/>
+      <c r="AG29" s="150"/>
+      <c r="AH29" s="151"/>
+    </row>
+    <row r="30" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V32" s="86"/>
+    </row>
     <row r="33" spans="2:2" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="154"/>
+      <c r="B33" s="99"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="24">
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="L5:P5"/>
     <mergeCell ref="R5:AH5"/>
@@ -5992,9 +7102,29 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:P29"/>
+    <mergeCell ref="R29:AH29"/>
+    <mergeCell ref="P7:P8"/>
   </mergeCells>
+  <conditionalFormatting sqref="B9:J25">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(_xludf.ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6018,15 +7148,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="13.8" x14ac:dyDescent="0.2">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="173" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="174" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="81" t="s">
@@ -6034,25 +7164,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="118"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="63" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="118"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="64" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="118"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="119"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="82" t="s">
         <v>56</v>
       </c>
@@ -6072,7 +7202,7 @@
       <c r="C11" s="65"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="117" t="s">
+      <c r="C12" s="174" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="81" t="s">
@@ -6080,43 +7210,43 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="118"/>
+      <c r="C13" s="175"/>
       <c r="D13" s="63" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="118"/>
+      <c r="C14" s="175"/>
       <c r="D14" s="61" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="118"/>
+      <c r="C15" s="175"/>
       <c r="D15" s="80" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="118"/>
+      <c r="C16" s="175"/>
       <c r="D16" s="61" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="118"/>
+      <c r="C17" s="175"/>
       <c r="D17" s="80" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="118"/>
+      <c r="C18" s="175"/>
       <c r="D18" s="61" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="119"/>
+      <c r="C19" s="176"/>
       <c r="D19" s="82" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Changement prime 5 et 6
</commit_message>
<xml_diff>
--- a/Excel_Exercice04_OperateursFonctionsCond.xlsx
+++ b/Excel_Exercice04_OperateursFonctionsCond.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilio\OneDrive\Bureau\École\Programmation\Outils et gestion\Remise-C13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2066A0EF-DB93-4572-A021-4BE7C8D294A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F268B76-BBF0-4705-9BAB-03140CEE3F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -323,7 +323,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1585,7 +1585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -1906,10 +1906,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -2022,6 +2018,118 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -2030,26 +2138,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -2074,69 +2162,81 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2162,125 +2262,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2315,10 +2326,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2644,7 +2651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="N1" zoomScale="112" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="U1" zoomScale="112" workbookViewId="0">
       <selection activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
@@ -2672,41 +2679,41 @@
   <sheetData>
     <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:34" ht="19.2" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="132"/>
-      <c r="O2" s="132"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="132"/>
-      <c r="R2" s="132"/>
-      <c r="S2" s="132"/>
-      <c r="T2" s="132"/>
-      <c r="U2" s="132"/>
-      <c r="V2" s="132"/>
-      <c r="W2" s="132"/>
-      <c r="X2" s="132"/>
-      <c r="Y2" s="132"/>
-      <c r="Z2" s="132"/>
-      <c r="AA2" s="132"/>
-      <c r="AB2" s="132"/>
-      <c r="AC2" s="132"/>
-      <c r="AD2" s="132"/>
-      <c r="AE2" s="132"/>
-      <c r="AF2" s="132"/>
-      <c r="AG2" s="132"/>
-      <c r="AH2" s="132"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="O2" s="125"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="125"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="125"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="125"/>
+      <c r="AB2" s="125"/>
+      <c r="AC2" s="125"/>
+      <c r="AD2" s="125"/>
+      <c r="AE2" s="125"/>
+      <c r="AF2" s="125"/>
+      <c r="AG2" s="125"/>
+      <c r="AH2" s="125"/>
     </row>
     <row r="3" spans="2:34" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -2717,122 +2724,122 @@
     </row>
     <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="L5" s="134" t="s">
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="L5" s="127" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="134"/>
-      <c r="N5" s="134"/>
-      <c r="O5" s="134"/>
-      <c r="P5" s="134"/>
-      <c r="R5" s="135" t="s">
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+      <c r="R5" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="135"/>
-      <c r="T5" s="135"/>
-      <c r="U5" s="135"/>
-      <c r="V5" s="135"/>
-      <c r="W5" s="135"/>
-      <c r="X5" s="135"/>
-      <c r="Y5" s="135"/>
-      <c r="Z5" s="135"/>
-      <c r="AA5" s="135"/>
-      <c r="AB5" s="135"/>
-      <c r="AC5" s="135"/>
-      <c r="AD5" s="135"/>
-      <c r="AE5" s="135"/>
-      <c r="AF5" s="135"/>
-      <c r="AG5" s="135"/>
-      <c r="AH5" s="135"/>
+      <c r="S5" s="131"/>
+      <c r="T5" s="131"/>
+      <c r="U5" s="131"/>
+      <c r="V5" s="131"/>
+      <c r="W5" s="131"/>
+      <c r="X5" s="131"/>
+      <c r="Y5" s="131"/>
+      <c r="Z5" s="131"/>
+      <c r="AA5" s="131"/>
+      <c r="AB5" s="131"/>
+      <c r="AC5" s="131"/>
+      <c r="AD5" s="131"/>
+      <c r="AE5" s="131"/>
+      <c r="AF5" s="131"/>
+      <c r="AG5" s="131"/>
+      <c r="AH5" s="131"/>
     </row>
     <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="142" t="s">
+      <c r="C7" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="144" t="s">
+      <c r="D7" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="136" t="s">
+      <c r="E7" s="132" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="146" t="s">
+      <c r="F7" s="144" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="138" t="s">
+      <c r="G7" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="139"/>
-      <c r="I7" s="119" t="s">
+      <c r="H7" s="135"/>
+      <c r="I7" s="146" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="120"/>
+      <c r="J7" s="147"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="140" t="s">
+      <c r="L7" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="141"/>
-      <c r="N7" s="140" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="141"/>
-      <c r="P7" s="128" t="s">
+      <c r="M7" s="137"/>
+      <c r="N7" s="136" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="137"/>
+      <c r="P7" s="150" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="121" t="s">
+      <c r="R7" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="122"/>
+      <c r="S7" s="139"/>
       <c r="T7" s="11"/>
-      <c r="U7" s="121" t="s">
+      <c r="U7" s="138" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="122"/>
-      <c r="W7" s="121" t="s">
+      <c r="V7" s="139"/>
+      <c r="W7" s="138" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="122"/>
-      <c r="Y7" s="121" t="s">
+      <c r="X7" s="139"/>
+      <c r="Y7" s="138" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="122"/>
-      <c r="AA7" s="121" t="s">
+      <c r="Z7" s="139"/>
+      <c r="AA7" s="138" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="122"/>
-      <c r="AC7" s="121" t="s">
+      <c r="AB7" s="139"/>
+      <c r="AC7" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="122"/>
-      <c r="AE7" s="121" t="s">
+      <c r="AD7" s="139"/>
+      <c r="AE7" s="138" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="122"/>
+      <c r="AF7" s="139"/>
       <c r="AG7" s="11"/>
-      <c r="AH7" s="130" t="s">
+      <c r="AH7" s="152" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="127"/>
-      <c r="C8" s="143"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="147"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="143"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="145"/>
       <c r="G8" s="13" t="s">
         <v>9</v>
       </c>
@@ -2858,7 +2865,7 @@
       <c r="O8" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="129"/>
+      <c r="P8" s="151"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="20" t="s">
         <v>9</v>
@@ -2904,7 +2911,7 @@
         <v>40</v>
       </c>
       <c r="AG8" s="12"/>
-      <c r="AH8" s="131"/>
+      <c r="AH8" s="153"/>
     </row>
     <row r="9" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="37" t="s">
@@ -4908,46 +4915,46 @@
       <c r="AH28" s="4"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B29" s="123" t="s">
+      <c r="B29" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="124"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="123" t="s">
+      <c r="C29" s="129"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="125"/>
-      <c r="G29" s="123" t="s">
+      <c r="F29" s="130"/>
+      <c r="G29" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="124"/>
-      <c r="I29" s="124"/>
-      <c r="J29" s="124"/>
-      <c r="K29" s="124"/>
-      <c r="L29" s="124"/>
-      <c r="M29" s="124"/>
-      <c r="N29" s="124"/>
-      <c r="O29" s="124"/>
-      <c r="P29" s="125"/>
-      <c r="R29" s="123" t="s">
+      <c r="H29" s="129"/>
+      <c r="I29" s="129"/>
+      <c r="J29" s="129"/>
+      <c r="K29" s="129"/>
+      <c r="L29" s="129"/>
+      <c r="M29" s="129"/>
+      <c r="N29" s="129"/>
+      <c r="O29" s="129"/>
+      <c r="P29" s="130"/>
+      <c r="R29" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="124"/>
-      <c r="T29" s="124"/>
-      <c r="U29" s="124"/>
-      <c r="V29" s="124"/>
-      <c r="W29" s="124"/>
-      <c r="X29" s="124"/>
-      <c r="Y29" s="124"/>
-      <c r="Z29" s="124"/>
-      <c r="AA29" s="124"/>
-      <c r="AB29" s="124"/>
-      <c r="AC29" s="124"/>
-      <c r="AD29" s="124"/>
-      <c r="AE29" s="124"/>
-      <c r="AF29" s="124"/>
-      <c r="AG29" s="124"/>
-      <c r="AH29" s="125"/>
+      <c r="S29" s="129"/>
+      <c r="T29" s="129"/>
+      <c r="U29" s="129"/>
+      <c r="V29" s="129"/>
+      <c r="W29" s="129"/>
+      <c r="X29" s="129"/>
+      <c r="Y29" s="129"/>
+      <c r="Z29" s="129"/>
+      <c r="AA29" s="129"/>
+      <c r="AB29" s="129"/>
+      <c r="AC29" s="129"/>
+      <c r="AD29" s="129"/>
+      <c r="AE29" s="129"/>
+      <c r="AF29" s="129"/>
+      <c r="AG29" s="129"/>
+      <c r="AH29" s="130"/>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="E31" s="8"/>
@@ -5260,6 +5267,16 @@
     <sortCondition ref="AL9"/>
   </sortState>
   <mergeCells count="26">
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="R29:AH29"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AH7:AH8"/>
     <mergeCell ref="B2:AH2"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="L5:P5"/>
@@ -5276,16 +5293,6 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="U7:V7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="R29:AH29"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AH7:AH8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="125" orientation="portrait" r:id="rId1"/>
@@ -5300,8 +5307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -5332,50 +5339,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:34" s="102" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
+    <row r="2" spans="1:34" s="101" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
-      <c r="Y2" s="104"/>
-      <c r="Z2" s="104"/>
-      <c r="AA2" s="104"/>
-      <c r="AB2" s="104"/>
-      <c r="AC2" s="104"/>
-      <c r="AD2" s="104"/>
-      <c r="AE2" s="104"/>
-      <c r="AF2" s="104"/>
-      <c r="AG2" s="104"/>
-      <c r="AH2" s="104"/>
-    </row>
-    <row r="3" spans="1:34" s="102" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="105" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="103"/>
+      <c r="AA2" s="103"/>
+      <c r="AB2" s="103"/>
+      <c r="AC2" s="103"/>
+      <c r="AD2" s="103"/>
+      <c r="AE2" s="103"/>
+      <c r="AF2" s="103"/>
+      <c r="AG2" s="103"/>
+      <c r="AH2" s="103"/>
+    </row>
+    <row r="3" spans="1:34" s="101" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="104" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:34" s="102" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="106"/>
+    <row r="4" spans="1:34" s="101" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="105"/>
     </row>
     <row r="5" spans="1:34" ht="16.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="154" t="s">
@@ -5416,7 +5423,7 @@
       <c r="AG5" s="159"/>
       <c r="AH5" s="159"/>
     </row>
-    <row r="6" spans="1:34" s="102" customFormat="1" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:34" s="101" customFormat="1" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="87"/>
       <c r="B7" s="162" t="s">
@@ -5450,40 +5457,40 @@
         <v>0</v>
       </c>
       <c r="O7" s="172"/>
-      <c r="P7" s="152" t="s">
+      <c r="P7" s="177" t="s">
         <v>42</v>
       </c>
-      <c r="R7" s="148" t="s">
+      <c r="R7" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="148"/>
-      <c r="T7" s="116"/>
-      <c r="U7" s="148" t="s">
+      <c r="S7" s="173"/>
+      <c r="T7" s="115"/>
+      <c r="U7" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="148"/>
-      <c r="W7" s="148" t="s">
+      <c r="V7" s="173"/>
+      <c r="W7" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="148"/>
-      <c r="Y7" s="148" t="s">
+      <c r="X7" s="173"/>
+      <c r="Y7" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="148"/>
-      <c r="AA7" s="148" t="s">
+      <c r="Z7" s="173"/>
+      <c r="AA7" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="148"/>
-      <c r="AC7" s="148" t="s">
+      <c r="AB7" s="173"/>
+      <c r="AC7" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="148"/>
-      <c r="AE7" s="148" t="s">
+      <c r="AD7" s="173"/>
+      <c r="AE7" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="148"/>
-      <c r="AG7" s="116"/>
-      <c r="AH7" s="117" t="s">
+      <c r="AF7" s="173"/>
+      <c r="AG7" s="115"/>
+      <c r="AH7" s="116" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5494,158 +5501,177 @@
       <c r="D8" s="165"/>
       <c r="E8" s="167"/>
       <c r="F8" s="169"/>
-      <c r="G8" s="96" t="s">
+      <c r="G8" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="97" t="s">
+      <c r="H8" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="98" t="s">
+      <c r="I8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="97" t="s">
+      <c r="J8" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="115" t="s">
+      <c r="L8" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="115" t="s">
+      <c r="M8" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="115" t="s">
+      <c r="N8" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="115" t="s">
+      <c r="O8" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="153"/>
-      <c r="R8" s="113" t="s">
+      <c r="P8" s="178"/>
+      <c r="R8" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="S8" s="113" t="s">
+      <c r="S8" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="113"/>
-      <c r="U8" s="113" t="s">
+      <c r="T8" s="112"/>
+      <c r="U8" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="V8" s="113" t="s">
+      <c r="V8" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="W8" s="113" t="s">
+      <c r="W8" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="X8" s="113" t="s">
+      <c r="X8" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="Y8" s="113" t="s">
+      <c r="Y8" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="Z8" s="113" t="s">
+      <c r="Z8" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="AA8" s="113" t="s">
+      <c r="AA8" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="AB8" s="113" t="s">
+      <c r="AB8" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="AC8" s="113" t="s">
+      <c r="AC8" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="AD8" s="113" t="s">
+      <c r="AD8" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="AE8" s="113" t="s">
+      <c r="AE8" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="AF8" s="113" t="s">
+      <c r="AF8" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="AG8" s="113"/>
-      <c r="AH8" s="114"/>
+      <c r="AG8" s="112"/>
+      <c r="AH8" s="113"/>
     </row>
     <row r="9" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="87"/>
       <c r="B9" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="93">
+      <c r="D9" s="92">
         <v>38226</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="G9" s="94">
+      <c r="E9" s="183">
+        <f>YEARFRAC(D9,$B$31)</f>
+        <v>8.344444444444445</v>
+      </c>
+      <c r="F9" s="186">
+        <f>IF(MOD(E9,5) &gt;=0,ROUNDDOWN(E9/5+2,0),0)</f>
+        <v>3</v>
+      </c>
+      <c r="G9" s="93">
         <v>21.68</v>
       </c>
-      <c r="H9" s="95">
+      <c r="H9" s="94">
         <v>32.520000000000003</v>
       </c>
-      <c r="I9" s="94">
+      <c r="I9" s="93">
         <v>86639.77</v>
       </c>
-      <c r="J9" s="95">
+      <c r="J9" s="94">
         <v>138605.66</v>
       </c>
-      <c r="L9" s="100">
+      <c r="L9" s="185">
         <v>1837.5</v>
       </c>
-      <c r="M9" s="100">
+      <c r="M9" s="185">
         <v>12.7</v>
       </c>
-      <c r="N9" s="178">
+      <c r="N9" s="119">
         <v>87225.33</v>
       </c>
-      <c r="O9" s="178">
+      <c r="O9" s="119">
         <v>113521.61</v>
       </c>
-      <c r="P9" s="100">
+      <c r="P9" s="99">
         <v>6</v>
       </c>
-      <c r="R9" s="177">
+      <c r="R9" s="118">
         <f>L9*G9</f>
         <v>39837</v>
       </c>
-      <c r="S9" s="177">
+      <c r="S9" s="118">
         <f>M9*H9</f>
         <v>413.00400000000002</v>
       </c>
-      <c r="U9" s="100" t="s">
+      <c r="U9" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V9" s="177">
+      <c r="V9" s="118">
         <f>N9*0.01 +O9*0.015</f>
         <v>2575.0774499999998</v>
       </c>
-      <c r="W9" s="100" t="str">
+      <c r="W9" s="99" t="str">
         <f>IF(I9&lt;N9,"Oui","Non")</f>
         <v>Oui</v>
       </c>
-      <c r="X9" s="177" cm="1">
+      <c r="X9" s="118" cm="1">
         <f t="array" ref="X9">_xlfn.IFS(W9="Oui",((N9-I9)*0.1),W9="Non",0)</f>
         <v>58.55599999999977</v>
       </c>
-      <c r="Y9" s="100" t="str">
+      <c r="Y9" s="99" t="str">
         <f>IF(J9&lt;O9,"Oui","Non")</f>
         <v>Non</v>
       </c>
-      <c r="Z9" s="177" cm="1">
+      <c r="Z9" s="118" cm="1">
         <f t="array" ref="Z9">_xlfn.IFS(Y9="Oui",((O9-J9)*0.15),Y9="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AA9" s="100" t="str">
+      <c r="AA9" s="99" t="str">
         <f>IF(P9&gt;=6,"Oui","Non")</f>
         <v>Oui</v>
       </c>
-      <c r="AB9" s="177" cm="1">
+      <c r="AB9" s="118" cm="1">
         <f t="array" ref="AB9">_xlfn.IFS(AA9&gt;="Oui",(N9+O9)*0.0025,AA9="Non",0)</f>
         <v>501.86735000000004</v>
       </c>
-      <c r="AC9" s="100" t="str">
+      <c r="AC9" s="99" t="str">
         <f>IF(AND(Y9="Oui",W9="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AD9" s="85">
+        <f>IF(AND(W9="Oui",Y9="Oui"),(O9-J9)+(N9-I9)*(P9/100),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="85" t="str">
+        <f>IF(AND(P9&gt;=6)*OR('Données brutes'!W9="Oui",'Données brutes'!Y9="Oui"),"Oui","Non")</f>
+        <v>Oui</v>
+      </c>
+      <c r="AF9" s="85">
+        <f>IF(AE9="Oui",(15000/8)/(N9/O9),0)</f>
+        <v>2440.2661331289892</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5653,81 +5679,96 @@
       <c r="B10" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="91" t="s">
+      <c r="C10" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="93">
+      <c r="D10" s="92">
         <v>37601</v>
       </c>
-      <c r="E10" s="90"/>
-      <c r="G10" s="94">
+      <c r="E10" s="183">
+        <f t="shared" ref="E10:E25" si="0">YEARFRAC(D10,$B$31)</f>
+        <v>10.055555555555555</v>
+      </c>
+      <c r="F10" s="185">
+        <f t="shared" ref="F10:F25" si="1">IF(MOD(E10,5) &gt;=0,ROUNDDOWN(E10/5+2,0),0)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="93">
         <v>23.05</v>
       </c>
-      <c r="H10" s="95">
+      <c r="H10" s="94">
         <v>34.58</v>
       </c>
-      <c r="I10" s="94">
+      <c r="I10" s="93">
         <v>86104.49</v>
       </c>
-      <c r="J10" s="95">
+      <c r="J10" s="94">
         <v>141119.44</v>
       </c>
-      <c r="L10" s="100">
+      <c r="L10" s="185">
         <v>1800</v>
       </c>
-      <c r="M10" s="100">
+      <c r="M10" s="185">
         <v>25.2</v>
       </c>
-      <c r="N10" s="178">
+      <c r="N10" s="119">
         <v>100494.47</v>
       </c>
-      <c r="O10" s="178">
+      <c r="O10" s="119">
         <v>133202.71</v>
       </c>
-      <c r="P10" s="100">
+      <c r="P10" s="99">
         <v>2</v>
       </c>
-      <c r="R10" s="177">
-        <f t="shared" ref="R10:R25" si="0">L10*G10</f>
+      <c r="R10" s="118">
+        <f t="shared" ref="R10:R25" si="2">L10*G10</f>
         <v>41490</v>
       </c>
-      <c r="S10" s="177">
-        <f t="shared" ref="S10:S25" si="1">M10*H10</f>
+      <c r="S10" s="118">
+        <f t="shared" ref="S10:S25" si="3">M10*H10</f>
         <v>871.41599999999994</v>
       </c>
-      <c r="U10" s="100" t="s">
+      <c r="U10" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V10" s="177">
-        <f t="shared" ref="V10:V25" si="2">N10*0.01 +O10*0.015</f>
+      <c r="V10" s="118">
+        <f t="shared" ref="V10:V25" si="4">N10*0.01 +O10*0.015</f>
         <v>3002.9853499999999</v>
       </c>
-      <c r="W10" s="100" t="str">
-        <f t="shared" ref="W10:W25" si="3">IF(I10&lt;N10,"Oui","Non")</f>
-        <v>Oui</v>
-      </c>
-      <c r="X10" s="177" cm="1">
+      <c r="W10" s="99" t="str">
+        <f t="shared" ref="W10:W25" si="5">IF(I10&lt;N10,"Oui","Non")</f>
+        <v>Oui</v>
+      </c>
+      <c r="X10" s="118" cm="1">
         <f t="array" ref="X10">_xlfn.IFS(W10="Oui",((N10-I10)*0.1),W10="Non",0)</f>
         <v>1438.9979999999996</v>
       </c>
-      <c r="Y10" s="100" t="str">
-        <f t="shared" ref="Y10:Y25" si="4">IF(J10&lt;O10,"Oui","Non")</f>
-        <v>Non</v>
-      </c>
-      <c r="Z10" s="177" cm="1">
+      <c r="Y10" s="99" t="str">
+        <f t="shared" ref="Y10:Y25" si="6">IF(J10&lt;O10,"Oui","Non")</f>
+        <v>Non</v>
+      </c>
+      <c r="Z10" s="118" cm="1">
         <f t="array" ref="Z10">_xlfn.IFS(Y10="Oui",((O10-J10)*0.15),Y10="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AA10" s="100" t="str">
-        <f t="shared" ref="AA10:AA25" si="5">IF(P10&gt;=6,"Oui","Non")</f>
-        <v>Non</v>
-      </c>
-      <c r="AB10" s="177" cm="1">
+      <c r="AA10" s="99" t="str">
+        <f t="shared" ref="AA10:AA25" si="7">IF(P10&gt;=6,"Oui","Non")</f>
+        <v>Non</v>
+      </c>
+      <c r="AB10" s="118" cm="1">
         <f t="array" ref="AB10">_xlfn.IFS(AA10&gt;="Oui",(N10+O10)*0.0025,AA10="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AC10" s="100" t="str">
-        <f t="shared" ref="AC10:AC25" si="6">IF(AND(Y10="Oui",W10="Oui"),"Oui","Non")</f>
+      <c r="AC10" s="99" t="str">
+        <f t="shared" ref="AC10:AC25" si="8">IF(AND(Y10="Oui",W10="Oui"),"Oui","Non")</f>
+        <v>Non</v>
+      </c>
+      <c r="AD10" s="85">
+        <f t="shared" ref="AD10:AD25" si="9">IF(AND(W10="Oui",Y10="Oui"),(O10-J10)+(N10-I10)*(P10/100),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE10" s="85" t="str">
+        <f>IF(AND(P10&gt;=6)*OR('Données brutes'!W10="Oui",'Données brutes'!Y10="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
@@ -5736,82 +5777,97 @@
       <c r="B11" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="91" t="s">
+      <c r="C11" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="93">
+      <c r="D11" s="92">
         <v>35826</v>
       </c>
-      <c r="E11" s="90"/>
-      <c r="G11" s="94">
+      <c r="E11" s="183">
+        <f t="shared" si="0"/>
+        <v>14.916666666666666</v>
+      </c>
+      <c r="F11" s="185">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G11" s="93">
         <v>26.94</v>
       </c>
-      <c r="H11" s="95">
+      <c r="H11" s="94">
         <v>40.409999999999997</v>
       </c>
-      <c r="I11" s="94">
+      <c r="I11" s="93">
         <v>89605.86</v>
       </c>
-      <c r="J11" s="95">
+      <c r="J11" s="94">
         <v>156292.04</v>
       </c>
-      <c r="L11" s="100">
+      <c r="L11" s="185">
         <v>1800</v>
       </c>
-      <c r="M11" s="100">
-        <v>0</v>
-      </c>
-      <c r="N11" s="178">
+      <c r="M11" s="185">
+        <v>0</v>
+      </c>
+      <c r="N11" s="119">
         <v>76821.77</v>
       </c>
-      <c r="O11" s="178">
+      <c r="O11" s="119">
         <v>158727.13</v>
       </c>
-      <c r="P11" s="100">
+      <c r="P11" s="99">
         <v>6</v>
       </c>
-      <c r="R11" s="177">
-        <f t="shared" si="0"/>
+      <c r="R11" s="118">
+        <f t="shared" si="2"/>
         <v>48492</v>
       </c>
-      <c r="S11" s="177">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U11" s="100" t="s">
+      <c r="S11" s="118">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V11" s="177">
-        <f t="shared" si="2"/>
+      <c r="V11" s="118">
+        <f t="shared" si="4"/>
         <v>3149.1246500000002</v>
       </c>
-      <c r="W11" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X11" s="177" cm="1">
+      <c r="W11" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X11" s="118" cm="1">
         <f t="array" ref="X11">_xlfn.IFS(W11="Oui",((N11-I11)*0.1),W11="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y11" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z11" s="177" cm="1">
+      <c r="Y11" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z11" s="118" cm="1">
         <f t="array" ref="Z11">_xlfn.IFS(Y11="Oui",((O11-J11)*0.15),Y11="Non",0)</f>
         <v>365.26349999999945</v>
       </c>
-      <c r="AA11" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Oui</v>
-      </c>
-      <c r="AB11" s="177" cm="1">
+      <c r="AA11" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB11" s="118" cm="1">
         <f t="array" ref="AB11">_xlfn.IFS(AA11&gt;="Oui",(N11+O11)*0.0025,AA11="Non",0)</f>
         <v>588.87225000000012</v>
       </c>
-      <c r="AC11" s="100" t="str">
-        <f t="shared" si="6"/>
-        <v>Non</v>
+      <c r="AC11" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD11" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE11" s="85" t="str">
+        <f>IF(AND(P11&gt;=6)*OR('Données brutes'!W11="Oui",'Données brutes'!Y11="Oui"),"Oui","Non")</f>
+        <v>Oui</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5819,82 +5875,97 @@
       <c r="B12" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="91" t="s">
+      <c r="C12" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="93">
+      <c r="D12" s="92">
         <v>35403</v>
       </c>
-      <c r="E12" s="90"/>
-      <c r="G12" s="94">
+      <c r="E12" s="183">
+        <f t="shared" si="0"/>
+        <v>16.074999999999999</v>
+      </c>
+      <c r="F12" s="185">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="93">
         <v>27.87</v>
       </c>
-      <c r="H12" s="95">
+      <c r="H12" s="94">
         <v>41.81</v>
       </c>
-      <c r="I12" s="94">
+      <c r="I12" s="93">
         <v>88556.09</v>
       </c>
-      <c r="J12" s="95">
+      <c r="J12" s="94">
         <v>156576.41</v>
       </c>
-      <c r="L12" s="100">
+      <c r="L12" s="185">
         <v>1762.5</v>
       </c>
-      <c r="M12" s="100">
-        <v>0</v>
-      </c>
-      <c r="N12" s="178">
+      <c r="M12" s="185">
+        <v>0</v>
+      </c>
+      <c r="N12" s="119">
         <v>77813.539999999994</v>
       </c>
-      <c r="O12" s="178">
+      <c r="O12" s="119">
         <v>170576.59</v>
       </c>
-      <c r="P12" s="100">
+      <c r="P12" s="99">
         <v>9</v>
       </c>
-      <c r="R12" s="177">
-        <f t="shared" si="0"/>
+      <c r="R12" s="118">
+        <f t="shared" si="2"/>
         <v>49120.875</v>
       </c>
-      <c r="S12" s="177">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U12" s="100" t="s">
+      <c r="S12" s="118">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U12" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V12" s="177">
-        <f t="shared" si="2"/>
+      <c r="V12" s="118">
+        <f t="shared" si="4"/>
         <v>3336.7842500000002</v>
       </c>
-      <c r="W12" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X12" s="177" cm="1">
+      <c r="W12" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X12" s="118" cm="1">
         <f t="array" ref="X12">_xlfn.IFS(W12="Oui",((N12-I12)*0.1),W12="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y12" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z12" s="177" cm="1">
+      <c r="Y12" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z12" s="118" cm="1">
         <f t="array" ref="Z12">_xlfn.IFS(Y12="Oui",((O12-J12)*0.15),Y12="Non",0)</f>
         <v>2100.0269999999987</v>
       </c>
-      <c r="AA12" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Oui</v>
-      </c>
-      <c r="AB12" s="177" cm="1">
+      <c r="AA12" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB12" s="118" cm="1">
         <f t="array" ref="AB12">_xlfn.IFS(AA12&gt;="Oui",(N12+O12)*0.0025,AA12="Non",0)</f>
         <v>620.975325</v>
       </c>
-      <c r="AC12" s="100" t="str">
-        <f t="shared" si="6"/>
-        <v>Non</v>
+      <c r="AC12" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD12" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE12" s="85" t="str">
+        <f>IF(AND(P12&gt;=6)*OR('Données brutes'!W12="Oui",'Données brutes'!Y12="Oui"),"Oui","Non")</f>
+        <v>Oui</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5902,81 +5973,96 @@
       <c r="B13" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="91" t="s">
+      <c r="C13" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="93">
+      <c r="D13" s="92">
         <v>33093</v>
       </c>
-      <c r="E13" s="90"/>
-      <c r="G13" s="94">
+      <c r="E13" s="183">
+        <f t="shared" si="0"/>
+        <v>22.397222222222222</v>
+      </c>
+      <c r="F13" s="185">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G13" s="93">
         <v>32.93</v>
       </c>
-      <c r="H13" s="95">
+      <c r="H13" s="94">
         <v>49.4</v>
       </c>
-      <c r="I13" s="94">
+      <c r="I13" s="93">
         <v>91038.77</v>
       </c>
-      <c r="J13" s="95">
+      <c r="J13" s="94">
         <v>172168.01</v>
       </c>
-      <c r="L13" s="100">
+      <c r="L13" s="185">
         <v>1725</v>
       </c>
-      <c r="M13" s="100">
+      <c r="M13" s="185">
         <v>39.57</v>
       </c>
-      <c r="N13" s="178">
+      <c r="N13" s="119">
         <v>96236.12</v>
       </c>
-      <c r="O13" s="178">
+      <c r="O13" s="119">
         <v>177509.88</v>
       </c>
-      <c r="P13" s="100">
+      <c r="P13" s="99">
         <v>7</v>
       </c>
-      <c r="R13" s="177">
-        <f t="shared" si="0"/>
+      <c r="R13" s="118">
+        <f t="shared" si="2"/>
         <v>56804.25</v>
       </c>
-      <c r="S13" s="177">
-        <f t="shared" si="1"/>
+      <c r="S13" s="118">
+        <f t="shared" si="3"/>
         <v>1954.758</v>
       </c>
-      <c r="U13" s="100" t="s">
+      <c r="U13" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V13" s="177">
-        <f t="shared" si="2"/>
+      <c r="V13" s="118">
+        <f t="shared" si="4"/>
         <v>3625.0093999999999</v>
       </c>
-      <c r="W13" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Oui</v>
-      </c>
-      <c r="X13" s="177" cm="1">
+      <c r="W13" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="X13" s="118" cm="1">
         <f t="array" ref="X13">_xlfn.IFS(W13="Oui",((N13-I13)*0.1),W13="Non",0)</f>
         <v>519.7349999999991</v>
       </c>
-      <c r="Y13" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z13" s="177" cm="1">
+      <c r="Y13" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z13" s="118" cm="1">
         <f t="array" ref="Z13">_xlfn.IFS(Y13="Oui",((O13-J13)*0.15),Y13="Non",0)</f>
         <v>801.28049999999928</v>
       </c>
-      <c r="AA13" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Oui</v>
-      </c>
-      <c r="AB13" s="177" cm="1">
+      <c r="AA13" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB13" s="118" cm="1">
         <f t="array" ref="AB13">_xlfn.IFS(AA13&gt;="Oui",(N13+O13)*0.0025,AA13="Non",0)</f>
         <v>684.36500000000001</v>
       </c>
-      <c r="AC13" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC13" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Oui</v>
+      </c>
+      <c r="AD13" s="85">
+        <f t="shared" si="9"/>
+        <v>5705.6844999999948</v>
+      </c>
+      <c r="AE13" s="85" t="str">
+        <f>IF(AND(P13&gt;=6)*OR('Données brutes'!W13="Oui",'Données brutes'!Y13="Oui"),"Oui","Non")</f>
         <v>Oui</v>
       </c>
     </row>
@@ -5985,81 +6071,96 @@
       <c r="B14" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="93">
+      <c r="D14" s="92">
         <v>37900</v>
       </c>
-      <c r="E14" s="90"/>
-      <c r="G14" s="94">
+      <c r="E14" s="183">
+        <f t="shared" si="0"/>
+        <v>9.2361111111111107</v>
+      </c>
+      <c r="F14" s="185">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G14" s="93">
         <v>22.4</v>
       </c>
-      <c r="H14" s="95">
+      <c r="H14" s="94">
         <v>33.6</v>
       </c>
-      <c r="I14" s="94">
+      <c r="I14" s="93">
         <v>87296.23</v>
       </c>
-      <c r="J14" s="95">
+      <c r="J14" s="94">
         <v>141450.34</v>
       </c>
-      <c r="L14" s="100">
+      <c r="L14" s="185">
         <v>1837.5</v>
       </c>
-      <c r="M14" s="100">
+      <c r="M14" s="185">
         <v>98.2</v>
       </c>
-      <c r="N14" s="178">
+      <c r="N14" s="119">
         <v>86363.33</v>
       </c>
-      <c r="O14" s="178">
+      <c r="O14" s="119">
         <v>120584.13</v>
       </c>
-      <c r="P14" s="100">
+      <c r="P14" s="99">
         <v>6</v>
       </c>
-      <c r="R14" s="177">
-        <f t="shared" si="0"/>
+      <c r="R14" s="118">
+        <f t="shared" si="2"/>
         <v>41160</v>
       </c>
-      <c r="S14" s="177">
-        <f t="shared" si="1"/>
+      <c r="S14" s="118">
+        <f t="shared" si="3"/>
         <v>3299.5200000000004</v>
       </c>
-      <c r="U14" s="100" t="s">
+      <c r="U14" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V14" s="177">
-        <f t="shared" si="2"/>
+      <c r="V14" s="118">
+        <f t="shared" si="4"/>
         <v>2672.39525</v>
       </c>
-      <c r="W14" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X14" s="177" cm="1">
+      <c r="W14" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X14" s="118" cm="1">
         <f t="array" ref="X14">_xlfn.IFS(W14="Oui",((N14-I14)*0.1),W14="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y14" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Non</v>
-      </c>
-      <c r="Z14" s="177" cm="1">
+      <c r="Y14" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+      <c r="Z14" s="118" cm="1">
         <f t="array" ref="Z14">_xlfn.IFS(Y14="Oui",((O14-J14)*0.15),Y14="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Oui</v>
-      </c>
-      <c r="AB14" s="177" cm="1">
+      <c r="AA14" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB14" s="118" cm="1">
         <f t="array" ref="AB14">_xlfn.IFS(AA14&gt;="Oui",(N14+O14)*0.0025,AA14="Non",0)</f>
         <v>517.36865000000012</v>
       </c>
-      <c r="AC14" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC14" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD14" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="85" t="str">
+        <f>IF(AND(P14&gt;=6)*OR('Données brutes'!W14="Oui",'Données brutes'!Y14="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
@@ -6068,82 +6169,97 @@
       <c r="B15" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="93">
+      <c r="D15" s="92">
         <v>35590</v>
       </c>
-      <c r="E15" s="90"/>
-      <c r="G15" s="94">
+      <c r="E15" s="183">
+        <f t="shared" si="0"/>
+        <v>15.561111111111112</v>
+      </c>
+      <c r="F15" s="185">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="93">
         <v>27.46</v>
       </c>
-      <c r="H15" s="95">
+      <c r="H15" s="94">
         <v>41.19</v>
       </c>
-      <c r="I15" s="94">
+      <c r="I15" s="93">
         <v>88194.9</v>
       </c>
-      <c r="J15" s="95">
+      <c r="J15" s="94">
         <v>155011.24</v>
       </c>
-      <c r="L15" s="100">
+      <c r="L15" s="185">
         <v>1762.5</v>
       </c>
-      <c r="M15" s="100">
+      <c r="M15" s="185">
         <v>244.14</v>
       </c>
-      <c r="N15" s="178">
+      <c r="N15" s="119">
         <v>98812.43</v>
       </c>
-      <c r="O15" s="178">
+      <c r="O15" s="119">
         <v>119521.7</v>
       </c>
-      <c r="P15" s="100">
+      <c r="P15" s="99">
         <v>6</v>
       </c>
-      <c r="R15" s="177">
-        <f t="shared" si="0"/>
+      <c r="R15" s="118">
+        <f t="shared" si="2"/>
         <v>48398.25</v>
       </c>
-      <c r="S15" s="177">
-        <f t="shared" si="1"/>
+      <c r="S15" s="118">
+        <f t="shared" si="3"/>
         <v>10056.1266</v>
       </c>
-      <c r="U15" s="100" t="s">
+      <c r="U15" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V15" s="177">
-        <f t="shared" si="2"/>
+      <c r="V15" s="118">
+        <f t="shared" si="4"/>
         <v>2780.9497999999999</v>
       </c>
-      <c r="W15" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Oui</v>
-      </c>
-      <c r="X15" s="177" cm="1">
+      <c r="W15" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="X15" s="118" cm="1">
         <f t="array" ref="X15">_xlfn.IFS(W15="Oui",((N15-I15)*0.1),W15="Non",0)</f>
         <v>1061.7529999999999</v>
       </c>
-      <c r="Y15" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Non</v>
-      </c>
-      <c r="Z15" s="177" cm="1">
+      <c r="Y15" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+      <c r="Z15" s="118" cm="1">
         <f t="array" ref="Z15">_xlfn.IFS(Y15="Oui",((O15-J15)*0.15),Y15="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AA15" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Oui</v>
-      </c>
-      <c r="AB15" s="177" cm="1">
+      <c r="AA15" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB15" s="118" cm="1">
         <f t="array" ref="AB15">_xlfn.IFS(AA15&gt;="Oui",(N15+O15)*0.0025,AA15="Non",0)</f>
         <v>545.83532500000001</v>
       </c>
-      <c r="AC15" s="100" t="str">
-        <f t="shared" si="6"/>
-        <v>Non</v>
+      <c r="AC15" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD15" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE15" s="85" t="str">
+        <f>IF(AND(P15&gt;=6)*OR('Données brutes'!W15="Oui",'Données brutes'!Y15="Oui"),"Oui","Non")</f>
+        <v>Oui</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6151,82 +6267,97 @@
       <c r="B16" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="91" t="s">
+      <c r="C16" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="93">
+      <c r="D16" s="92">
         <v>35192</v>
       </c>
-      <c r="E16" s="90"/>
-      <c r="G16" s="94">
+      <c r="E16" s="183">
+        <f t="shared" si="0"/>
+        <v>16.649999999999999</v>
+      </c>
+      <c r="F16" s="185">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="93">
         <v>28.33</v>
       </c>
-      <c r="H16" s="95">
+      <c r="H16" s="94">
         <v>42.5</v>
       </c>
-      <c r="I16" s="94">
+      <c r="I16" s="93">
         <v>88963.64</v>
       </c>
-      <c r="J16" s="95">
+      <c r="J16" s="94">
         <v>158342.45000000001</v>
       </c>
-      <c r="L16" s="100">
+      <c r="L16" s="185">
         <v>1762.5</v>
       </c>
-      <c r="M16" s="100">
+      <c r="M16" s="185">
         <v>109.39</v>
       </c>
-      <c r="N16" s="178">
+      <c r="N16" s="119">
         <v>89879.18</v>
       </c>
-      <c r="O16" s="178">
+      <c r="O16" s="119">
         <v>164850.17000000001</v>
       </c>
-      <c r="P16" s="100">
+      <c r="P16" s="99">
         <v>4</v>
       </c>
-      <c r="R16" s="177">
-        <f t="shared" si="0"/>
+      <c r="R16" s="118">
+        <f t="shared" si="2"/>
         <v>49931.625</v>
       </c>
-      <c r="S16" s="177">
-        <f t="shared" si="1"/>
+      <c r="S16" s="118">
+        <f t="shared" si="3"/>
         <v>4649.0749999999998</v>
       </c>
-      <c r="U16" s="100" t="s">
+      <c r="U16" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V16" s="177">
-        <f t="shared" si="2"/>
+      <c r="V16" s="118">
+        <f t="shared" si="4"/>
         <v>3371.5443500000001</v>
       </c>
-      <c r="W16" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Oui</v>
-      </c>
-      <c r="X16" s="177" cm="1">
+      <c r="W16" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="X16" s="118" cm="1">
         <f t="array" ref="X16">_xlfn.IFS(W16="Oui",((N16-I16)*0.1),W16="Non",0)</f>
         <v>91.553999999999363</v>
       </c>
-      <c r="Y16" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z16" s="177" cm="1">
+      <c r="Y16" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z16" s="118" cm="1">
         <f t="array" ref="Z16">_xlfn.IFS(Y16="Oui",((O16-J16)*0.15),Y16="Non",0)</f>
         <v>976.15800000000013</v>
       </c>
-      <c r="AA16" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Non</v>
-      </c>
-      <c r="AB16" s="177" cm="1">
+      <c r="AA16" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Non</v>
+      </c>
+      <c r="AB16" s="118" cm="1">
         <f t="array" ref="AB16">_xlfn.IFS(AA16&gt;="Oui",(N16+O16)*0.0025,AA16="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AC16" s="100" t="str">
-        <f t="shared" si="6"/>
-        <v>Oui</v>
+      <c r="AC16" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Oui</v>
+      </c>
+      <c r="AD16" s="85">
+        <f t="shared" si="9"/>
+        <v>6544.3416000000007</v>
+      </c>
+      <c r="AE16" s="85" t="str">
+        <f>IF(AND(P16&gt;=6)*OR('Données brutes'!W16="Oui",'Données brutes'!Y16="Oui"),"Oui","Non")</f>
+        <v>Non</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6234,81 +6365,96 @@
       <c r="B17" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="91" t="s">
+      <c r="C17" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="93">
+      <c r="D17" s="92">
         <v>36628</v>
       </c>
-      <c r="E17" s="90"/>
-      <c r="G17" s="94">
+      <c r="E17" s="183">
+        <f t="shared" si="0"/>
+        <v>12.719444444444445</v>
+      </c>
+      <c r="F17" s="185">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G17" s="93">
         <v>25.19</v>
       </c>
-      <c r="H17" s="95">
+      <c r="H17" s="94">
         <v>37.78</v>
       </c>
-      <c r="I17" s="94">
+      <c r="I17" s="93">
         <v>88023.83</v>
       </c>
-      <c r="J17" s="95">
+      <c r="J17" s="94">
         <v>149436.59</v>
       </c>
-      <c r="L17" s="100">
+      <c r="L17" s="185">
         <v>1800</v>
       </c>
-      <c r="M17" s="100">
-        <v>0</v>
-      </c>
-      <c r="N17" s="178">
+      <c r="M17" s="185">
+        <v>0</v>
+      </c>
+      <c r="N17" s="119">
         <v>92616.29</v>
       </c>
-      <c r="O17" s="178">
+      <c r="O17" s="119">
         <v>149766.94</v>
       </c>
-      <c r="P17" s="100">
+      <c r="P17" s="99">
         <v>9</v>
       </c>
-      <c r="R17" s="177">
-        <f t="shared" si="0"/>
+      <c r="R17" s="118">
+        <f t="shared" si="2"/>
         <v>45342</v>
       </c>
-      <c r="S17" s="177">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U17" s="100" t="s">
+      <c r="S17" s="118">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V17" s="177">
-        <f t="shared" si="2"/>
+      <c r="V17" s="118">
+        <f t="shared" si="4"/>
         <v>3172.6669999999999</v>
       </c>
-      <c r="W17" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Oui</v>
-      </c>
-      <c r="X17" s="177" cm="1">
+      <c r="W17" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="X17" s="118" cm="1">
         <f t="array" ref="X17">_xlfn.IFS(W17="Oui",((N17-I17)*0.1),W17="Non",0)</f>
         <v>459.24599999999919</v>
       </c>
-      <c r="Y17" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z17" s="177" cm="1">
+      <c r="Y17" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z17" s="118" cm="1">
         <f t="array" ref="Z17">_xlfn.IFS(Y17="Oui",((O17-J17)*0.15),Y17="Non",0)</f>
         <v>49.552500000000869</v>
       </c>
-      <c r="AA17" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Oui</v>
-      </c>
-      <c r="AB17" s="177" cm="1">
+      <c r="AA17" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB17" s="118" cm="1">
         <f t="array" ref="AB17">_xlfn.IFS(AA17&gt;="Oui",(N17+O17)*0.0025,AA17="Non",0)</f>
         <v>605.95807500000001</v>
       </c>
-      <c r="AC17" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC17" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Oui</v>
+      </c>
+      <c r="AD17" s="85">
+        <f t="shared" si="9"/>
+        <v>743.67140000000506</v>
+      </c>
+      <c r="AE17" s="85" t="str">
+        <f>IF(AND(P17&gt;=6)*OR('Données brutes'!W17="Oui",'Données brutes'!Y17="Oui"),"Oui","Non")</f>
         <v>Oui</v>
       </c>
     </row>
@@ -6317,81 +6463,96 @@
       <c r="B18" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="91" t="s">
+      <c r="C18" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="93">
+      <c r="D18" s="92">
         <v>30115</v>
       </c>
-      <c r="E18" s="90"/>
-      <c r="G18" s="94">
+      <c r="E18" s="183">
+        <f t="shared" si="0"/>
+        <v>30.55</v>
+      </c>
+      <c r="F18" s="185">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G18" s="93">
         <v>39.46</v>
       </c>
-      <c r="H18" s="95">
+      <c r="H18" s="94">
         <v>59.19</v>
       </c>
-      <c r="I18" s="94">
+      <c r="I18" s="93">
         <v>92465.44</v>
       </c>
-      <c r="J18" s="95">
+      <c r="J18" s="94">
         <v>188016.91</v>
       </c>
-      <c r="L18" s="100">
+      <c r="L18" s="185">
         <v>1650</v>
       </c>
-      <c r="M18" s="100">
+      <c r="M18" s="185">
         <v>143.27000000000001</v>
       </c>
-      <c r="N18" s="178">
+      <c r="N18" s="119">
         <v>86538.68</v>
       </c>
-      <c r="O18" s="178">
+      <c r="O18" s="119">
         <v>168507.1</v>
       </c>
-      <c r="P18" s="100">
+      <c r="P18" s="99">
         <v>5</v>
       </c>
-      <c r="R18" s="177">
-        <f t="shared" si="0"/>
+      <c r="R18" s="118">
+        <f t="shared" si="2"/>
         <v>65109</v>
       </c>
-      <c r="S18" s="177">
-        <f t="shared" si="1"/>
+      <c r="S18" s="118">
+        <f t="shared" si="3"/>
         <v>8480.1512999999995</v>
       </c>
-      <c r="U18" s="100" t="s">
+      <c r="U18" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V18" s="177">
-        <f t="shared" si="2"/>
+      <c r="V18" s="118">
+        <f t="shared" si="4"/>
         <v>3392.9933000000001</v>
       </c>
-      <c r="W18" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X18" s="177" cm="1">
+      <c r="W18" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X18" s="118" cm="1">
         <f t="array" ref="X18">_xlfn.IFS(W18="Oui",((N18-I18)*0.1),W18="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y18" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Non</v>
-      </c>
-      <c r="Z18" s="177" cm="1">
+      <c r="Y18" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+      <c r="Z18" s="118" cm="1">
         <f t="array" ref="Z18">_xlfn.IFS(Y18="Oui",((O18-J18)*0.15),Y18="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AA18" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Non</v>
-      </c>
-      <c r="AB18" s="177" cm="1">
+      <c r="AA18" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Non</v>
+      </c>
+      <c r="AB18" s="118" cm="1">
         <f t="array" ref="AB18">_xlfn.IFS(AA18&gt;="Oui",(N18+O18)*0.0025,AA18="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AC18" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC18" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD18" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE18" s="85" t="str">
+        <f>IF(AND(P18&gt;=6)*OR('Données brutes'!W18="Oui",'Données brutes'!Y18="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
@@ -6400,81 +6561,96 @@
       <c r="B19" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="93">
+      <c r="D19" s="92">
         <v>41231</v>
       </c>
-      <c r="E19" s="90"/>
-      <c r="G19" s="94">
+      <c r="E19" s="183">
+        <f t="shared" si="0"/>
+        <v>0.11944444444444445</v>
+      </c>
+      <c r="F19" s="185">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G19" s="93">
         <v>15.1</v>
       </c>
-      <c r="H19" s="95">
+      <c r="H19" s="94">
         <v>22.64</v>
       </c>
-      <c r="I19" s="94">
+      <c r="I19" s="93">
         <v>82233.27</v>
       </c>
-      <c r="J19" s="95">
+      <c r="J19" s="94">
         <v>114677.5</v>
       </c>
-      <c r="L19" s="100">
+      <c r="L19" s="185">
         <v>1875</v>
       </c>
-      <c r="M19" s="100">
-        <v>0</v>
-      </c>
-      <c r="N19" s="178">
+      <c r="M19" s="185">
+        <v>0</v>
+      </c>
+      <c r="N19" s="119">
         <v>74240.86</v>
       </c>
-      <c r="O19" s="178">
+      <c r="O19" s="119">
         <v>112740.09</v>
       </c>
-      <c r="P19" s="100">
+      <c r="P19" s="99">
         <v>5</v>
       </c>
-      <c r="R19" s="177">
-        <f t="shared" si="0"/>
+      <c r="R19" s="118">
+        <f t="shared" si="2"/>
         <v>28312.5</v>
       </c>
-      <c r="S19" s="177">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U19" s="100" t="s">
+      <c r="S19" s="118">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V19" s="177">
-        <f t="shared" si="2"/>
+      <c r="V19" s="118">
+        <f t="shared" si="4"/>
         <v>2433.5099499999997</v>
       </c>
-      <c r="W19" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X19" s="177" cm="1">
+      <c r="W19" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X19" s="118" cm="1">
         <f t="array" ref="X19">_xlfn.IFS(W19="Oui",((N19-I19)*0.1),W19="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y19" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Non</v>
-      </c>
-      <c r="Z19" s="177" cm="1">
+      <c r="Y19" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+      <c r="Z19" s="118" cm="1">
         <f t="array" ref="Z19">_xlfn.IFS(Y19="Oui",((O19-J19)*0.15),Y19="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AA19" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Non</v>
-      </c>
-      <c r="AB19" s="177" cm="1">
+      <c r="AA19" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Non</v>
+      </c>
+      <c r="AB19" s="118" cm="1">
         <f t="array" ref="AB19">_xlfn.IFS(AA19&gt;="Oui",(N19+O19)*0.0025,AA19="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AC19" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC19" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD19" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE19" s="85" t="str">
+        <f>IF(AND(P19&gt;=6)*OR('Données brutes'!W19="Oui",'Données brutes'!Y19="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
@@ -6483,82 +6659,97 @@
       <c r="B20" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="91" t="s">
+      <c r="C20" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="93">
+      <c r="D20" s="92">
         <v>31824</v>
       </c>
-      <c r="E20" s="90"/>
-      <c r="G20" s="94">
+      <c r="E20" s="183">
+        <f t="shared" si="0"/>
+        <v>25.875</v>
+      </c>
+      <c r="F20" s="185">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G20" s="93">
         <v>35.71</v>
       </c>
-      <c r="H20" s="95">
+      <c r="H20" s="94">
         <v>53.57</v>
       </c>
-      <c r="I20" s="94">
+      <c r="I20" s="93">
         <v>91406.45</v>
       </c>
-      <c r="J20" s="95">
+      <c r="J20" s="94">
         <v>178594.61</v>
       </c>
-      <c r="L20" s="100">
+      <c r="L20" s="185">
         <v>1687.5</v>
       </c>
-      <c r="M20" s="100">
+      <c r="M20" s="185">
         <v>145.13</v>
       </c>
-      <c r="N20" s="178">
+      <c r="N20" s="119">
         <v>90744.11</v>
       </c>
-      <c r="O20" s="178">
+      <c r="O20" s="119">
         <v>180217.79</v>
       </c>
-      <c r="P20" s="100">
+      <c r="P20" s="99">
         <v>9</v>
       </c>
-      <c r="R20" s="177">
-        <f t="shared" si="0"/>
+      <c r="R20" s="118">
+        <f t="shared" si="2"/>
         <v>60260.625</v>
       </c>
-      <c r="S20" s="177">
-        <f t="shared" si="1"/>
+      <c r="S20" s="118">
+        <f t="shared" si="3"/>
         <v>7774.6140999999998</v>
       </c>
-      <c r="U20" s="100" t="s">
+      <c r="U20" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V20" s="177">
-        <f t="shared" si="2"/>
+      <c r="V20" s="118">
+        <f t="shared" si="4"/>
         <v>3610.70795</v>
       </c>
-      <c r="W20" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X20" s="177" cm="1">
+      <c r="W20" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X20" s="118" cm="1">
         <f t="array" ref="X20">_xlfn.IFS(W20="Oui",((N20-I20)*0.1),W20="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y20" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z20" s="177" cm="1">
+      <c r="Y20" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z20" s="118" cm="1">
         <f t="array" ref="Z20">_xlfn.IFS(Y20="Oui",((O20-J20)*0.15),Y20="Non",0)</f>
         <v>243.4770000000033</v>
       </c>
-      <c r="AA20" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Oui</v>
-      </c>
-      <c r="AB20" s="177" cm="1">
+      <c r="AA20" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB20" s="118" cm="1">
         <f t="array" ref="AB20">_xlfn.IFS(AA20&gt;="Oui",(N20+O20)*0.0025,AA20="Non",0)</f>
         <v>677.40475000000004</v>
       </c>
-      <c r="AC20" s="100" t="str">
-        <f t="shared" si="6"/>
-        <v>Non</v>
+      <c r="AC20" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD20" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE20" s="85" t="str">
+        <f>IF(AND(P20&gt;=6)*OR('Données brutes'!W20="Oui",'Données brutes'!Y20="Oui"),"Oui","Non")</f>
+        <v>Oui</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6566,81 +6757,96 @@
       <c r="B21" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="91" t="s">
+      <c r="C21" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="93">
+      <c r="D21" s="92">
         <v>38150</v>
       </c>
-      <c r="E21" s="90"/>
-      <c r="G21" s="94">
+      <c r="E21" s="183">
+        <f t="shared" si="0"/>
+        <v>8.5527777777777771</v>
+      </c>
+      <c r="F21" s="185">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G21" s="93">
         <v>21.85</v>
       </c>
-      <c r="H21" s="95">
+      <c r="H21" s="94">
         <v>32.770000000000003</v>
       </c>
-      <c r="I21" s="94">
+      <c r="I21" s="93">
         <v>86792.81</v>
       </c>
-      <c r="J21" s="95">
+      <c r="J21" s="94">
         <v>139268.84</v>
       </c>
-      <c r="L21" s="100">
+      <c r="L21" s="185">
         <v>1837.5</v>
       </c>
-      <c r="M21" s="100">
+      <c r="M21" s="185">
         <v>191.85</v>
       </c>
-      <c r="N21" s="178">
+      <c r="N21" s="119">
         <v>92277.83</v>
       </c>
-      <c r="O21" s="178">
+      <c r="O21" s="119">
         <v>139124.15</v>
       </c>
-      <c r="P21" s="100">
+      <c r="P21" s="99">
         <v>3</v>
       </c>
-      <c r="R21" s="177">
-        <f t="shared" si="0"/>
+      <c r="R21" s="118">
+        <f t="shared" si="2"/>
         <v>40149.375</v>
       </c>
-      <c r="S21" s="177">
-        <f t="shared" si="1"/>
+      <c r="S21" s="118">
+        <f t="shared" si="3"/>
         <v>6286.9245000000001</v>
       </c>
-      <c r="U21" s="100" t="s">
+      <c r="U21" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V21" s="177">
-        <f t="shared" si="2"/>
+      <c r="V21" s="118">
+        <f t="shared" si="4"/>
         <v>3009.6405499999996</v>
       </c>
-      <c r="W21" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Oui</v>
-      </c>
-      <c r="X21" s="177" cm="1">
+      <c r="W21" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="X21" s="118" cm="1">
         <f t="array" ref="X21">_xlfn.IFS(W21="Oui",((N21-I21)*0.1),W21="Non",0)</f>
         <v>548.50200000000041</v>
       </c>
-      <c r="Y21" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Non</v>
-      </c>
-      <c r="Z21" s="177" cm="1">
+      <c r="Y21" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+      <c r="Z21" s="118" cm="1">
         <f t="array" ref="Z21">_xlfn.IFS(Y21="Oui",((O21-J21)*0.15),Y21="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Non</v>
-      </c>
-      <c r="AB21" s="177" cm="1">
+      <c r="AA21" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Non</v>
+      </c>
+      <c r="AB21" s="118" cm="1">
         <f t="array" ref="AB21">_xlfn.IFS(AA21&gt;="Oui",(N21+O21)*0.0025,AA21="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AC21" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC21" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD21" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="85" t="str">
+        <f>IF(AND(P21&gt;=6)*OR('Données brutes'!W21="Oui",'Données brutes'!Y21="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
@@ -6649,81 +6855,96 @@
       <c r="B22" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="91" t="s">
+      <c r="C22" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="93">
+      <c r="D22" s="92">
         <v>32891</v>
       </c>
-      <c r="E22" s="90"/>
-      <c r="G22" s="94">
+      <c r="E22" s="183">
+        <f t="shared" si="0"/>
+        <v>22.952777777777779</v>
+      </c>
+      <c r="F22" s="185">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G22" s="93">
         <v>33.380000000000003</v>
       </c>
-      <c r="H22" s="95">
+      <c r="H22" s="94">
         <v>50.06</v>
       </c>
-      <c r="I22" s="94">
+      <c r="I22" s="93">
         <v>91420.63</v>
       </c>
-      <c r="J22" s="95">
+      <c r="J22" s="94">
         <v>173822.75</v>
       </c>
-      <c r="L22" s="100">
+      <c r="L22" s="185">
         <v>1725</v>
       </c>
-      <c r="M22" s="100">
+      <c r="M22" s="185">
         <v>150.72</v>
       </c>
-      <c r="N22" s="178">
+      <c r="N22" s="119">
         <v>80527.14</v>
       </c>
-      <c r="O22" s="178">
+      <c r="O22" s="119">
         <v>181545.58</v>
       </c>
-      <c r="P22" s="100">
+      <c r="P22" s="99">
         <v>5</v>
       </c>
-      <c r="R22" s="177">
-        <f t="shared" si="0"/>
+      <c r="R22" s="118">
+        <f t="shared" si="2"/>
         <v>57580.500000000007</v>
       </c>
-      <c r="S22" s="177">
-        <f t="shared" si="1"/>
+      <c r="S22" s="118">
+        <f t="shared" si="3"/>
         <v>7545.0432000000001</v>
       </c>
-      <c r="U22" s="100" t="s">
+      <c r="U22" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V22" s="177">
-        <f t="shared" si="2"/>
+      <c r="V22" s="118">
+        <f t="shared" si="4"/>
         <v>3528.4550999999997</v>
       </c>
-      <c r="W22" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X22" s="177" cm="1">
+      <c r="W22" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X22" s="118" cm="1">
         <f t="array" ref="X22">_xlfn.IFS(W22="Oui",((N22-I22)*0.1),W22="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y22" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z22" s="177" cm="1">
+      <c r="Y22" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z22" s="118" cm="1">
         <f t="array" ref="Z22">_xlfn.IFS(Y22="Oui",((O22-J22)*0.15),Y22="Non",0)</f>
         <v>1158.424499999998</v>
       </c>
-      <c r="AA22" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Non</v>
-      </c>
-      <c r="AB22" s="177" cm="1">
+      <c r="AA22" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Non</v>
+      </c>
+      <c r="AB22" s="118" cm="1">
         <f t="array" ref="AB22">_xlfn.IFS(AA22&gt;="Oui",(N22+O22)*0.0025,AA22="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AC22" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC22" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD22" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE22" s="85" t="str">
+        <f>IF(AND(P22&gt;=6)*OR('Données brutes'!W22="Oui",'Données brutes'!Y22="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
@@ -6732,82 +6953,97 @@
       <c r="B23" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="91" t="s">
+      <c r="C23" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="93">
+      <c r="D23" s="92">
         <v>41102</v>
       </c>
-      <c r="E23" s="90"/>
-      <c r="G23" s="94">
+      <c r="E23" s="183">
+        <f t="shared" si="0"/>
+        <v>0.46944444444444444</v>
+      </c>
+      <c r="F23" s="185">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G23" s="93">
         <v>15.38</v>
       </c>
-      <c r="H23" s="95">
+      <c r="H23" s="94">
         <v>23.07</v>
       </c>
-      <c r="I23" s="94">
+      <c r="I23" s="93">
         <v>82498.34</v>
       </c>
-      <c r="J23" s="95">
+      <c r="J23" s="94">
         <v>115826.13</v>
       </c>
-      <c r="L23" s="100">
+      <c r="L23" s="185">
         <v>1875</v>
       </c>
-      <c r="M23" s="100">
+      <c r="M23" s="185">
         <v>159.16999999999999</v>
       </c>
-      <c r="N23" s="178">
+      <c r="N23" s="119">
         <v>73878.58</v>
       </c>
-      <c r="O23" s="178">
+      <c r="O23" s="119">
         <v>125469.62</v>
       </c>
-      <c r="P23" s="100">
+      <c r="P23" s="99">
         <v>9</v>
       </c>
-      <c r="R23" s="177">
-        <f t="shared" si="0"/>
+      <c r="R23" s="118">
+        <f t="shared" si="2"/>
         <v>28837.5</v>
       </c>
-      <c r="S23" s="177">
-        <f t="shared" si="1"/>
+      <c r="S23" s="118">
+        <f t="shared" si="3"/>
         <v>3672.0518999999999</v>
       </c>
-      <c r="U23" s="100" t="s">
+      <c r="U23" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V23" s="177">
-        <f t="shared" si="2"/>
+      <c r="V23" s="118">
+        <f t="shared" si="4"/>
         <v>2620.8300999999997</v>
       </c>
-      <c r="W23" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X23" s="177" cm="1">
+      <c r="W23" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X23" s="118" cm="1">
         <f t="array" ref="X23">_xlfn.IFS(W23="Oui",((N23-I23)*0.1),W23="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y23" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z23" s="177" cm="1">
+      <c r="Y23" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z23" s="118" cm="1">
         <f t="array" ref="Z23">_xlfn.IFS(Y23="Oui",((O23-J23)*0.15),Y23="Non",0)</f>
         <v>1446.5234999999986</v>
       </c>
-      <c r="AA23" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Oui</v>
-      </c>
-      <c r="AB23" s="177" cm="1">
+      <c r="AA23" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Oui</v>
+      </c>
+      <c r="AB23" s="118" cm="1">
         <f t="array" ref="AB23">_xlfn.IFS(AA23&gt;="Oui",(N23+O23)*0.0025,AA23="Non",0)</f>
         <v>498.37050000000005</v>
       </c>
-      <c r="AC23" s="100" t="str">
-        <f t="shared" si="6"/>
-        <v>Non</v>
+      <c r="AC23" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD23" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE23" s="85" t="str">
+        <f>IF(AND(P23&gt;=6)*OR('Données brutes'!W23="Oui",'Données brutes'!Y23="Oui"),"Oui","Non")</f>
+        <v>Oui</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6815,81 +7051,96 @@
       <c r="B24" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="93">
+      <c r="D24" s="92">
         <v>29465</v>
       </c>
-      <c r="E24" s="90"/>
-      <c r="G24" s="94">
+      <c r="E24" s="183">
+        <f t="shared" si="0"/>
+        <v>32.333333333333336</v>
+      </c>
+      <c r="F24" s="185">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G24" s="93">
         <v>40.880000000000003</v>
       </c>
-      <c r="H24" s="95">
+      <c r="H24" s="94">
         <v>61.33</v>
       </c>
-      <c r="I24" s="94">
+      <c r="I24" s="93">
         <v>93640.78</v>
       </c>
-      <c r="J24" s="95">
+      <c r="J24" s="94">
         <v>193110.06</v>
       </c>
-      <c r="L24" s="100">
+      <c r="L24" s="185">
         <v>1650</v>
       </c>
-      <c r="M24" s="100">
-        <v>0</v>
-      </c>
-      <c r="N24" s="178">
+      <c r="M24" s="185">
+        <v>0</v>
+      </c>
+      <c r="N24" s="119">
         <v>83732.44</v>
       </c>
-      <c r="O24" s="178">
+      <c r="O24" s="119">
         <v>208951.82</v>
       </c>
-      <c r="P24" s="100">
+      <c r="P24" s="99">
         <v>2</v>
       </c>
-      <c r="R24" s="177">
-        <f t="shared" si="0"/>
+      <c r="R24" s="118">
+        <f t="shared" si="2"/>
         <v>67452</v>
       </c>
-      <c r="S24" s="177">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U24" s="100" t="s">
+      <c r="S24" s="118">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V24" s="177">
-        <f t="shared" si="2"/>
+      <c r="V24" s="118">
+        <f t="shared" si="4"/>
         <v>3971.6017000000002</v>
       </c>
-      <c r="W24" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Non</v>
-      </c>
-      <c r="X24" s="177" cm="1">
+      <c r="W24" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Non</v>
+      </c>
+      <c r="X24" s="118" cm="1">
         <f t="array" ref="X24">_xlfn.IFS(W24="Oui",((N24-I24)*0.1),W24="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="Y24" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Oui</v>
-      </c>
-      <c r="Z24" s="177" cm="1">
+      <c r="Y24" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Oui</v>
+      </c>
+      <c r="Z24" s="118" cm="1">
         <f t="array" ref="Z24">_xlfn.IFS(Y24="Oui",((O24-J24)*0.15),Y24="Non",0)</f>
         <v>2376.2640000000015</v>
       </c>
-      <c r="AA24" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Non</v>
-      </c>
-      <c r="AB24" s="177" cm="1">
+      <c r="AA24" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Non</v>
+      </c>
+      <c r="AB24" s="118" cm="1">
         <f t="array" ref="AB24">_xlfn.IFS(AA24&gt;="Oui",(N24+O24)*0.0025,AA24="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AC24" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC24" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD24" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="85" t="str">
+        <f>IF(AND(P24&gt;=6)*OR('Données brutes'!W24="Oui",'Données brutes'!Y24="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
@@ -6898,200 +7149,227 @@
       <c r="B25" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="93">
+      <c r="D25" s="92">
         <v>30711</v>
       </c>
-      <c r="E25" s="90"/>
-      <c r="G25" s="94">
+      <c r="E25" s="183">
+        <f t="shared" si="0"/>
+        <v>28.916666666666668</v>
+      </c>
+      <c r="F25" s="185">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G25" s="93">
         <v>38.15</v>
       </c>
-      <c r="H25" s="95">
+      <c r="H25" s="94">
         <v>57.23</v>
       </c>
-      <c r="I25" s="94">
+      <c r="I25" s="93">
         <v>93464.74</v>
       </c>
-      <c r="J25" s="95">
+      <c r="J25" s="94">
         <v>187513.86</v>
       </c>
-      <c r="L25" s="100">
+      <c r="L25" s="185">
         <v>1687.5</v>
       </c>
-      <c r="M25" s="100">
+      <c r="M25" s="185">
         <v>226.41</v>
       </c>
-      <c r="N25" s="178">
+      <c r="N25" s="119">
         <v>98278.63</v>
       </c>
-      <c r="O25" s="178">
+      <c r="O25" s="119">
         <v>171337.91</v>
       </c>
-      <c r="P25" s="100">
+      <c r="P25" s="99">
         <v>5</v>
       </c>
-      <c r="R25" s="177">
-        <f t="shared" si="0"/>
+      <c r="R25" s="118">
+        <f t="shared" si="2"/>
         <v>64378.125</v>
       </c>
-      <c r="S25" s="177">
-        <f t="shared" si="1"/>
+      <c r="S25" s="118">
+        <f t="shared" si="3"/>
         <v>12957.444299999999</v>
       </c>
-      <c r="U25" s="100" t="s">
+      <c r="U25" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="V25" s="177">
-        <f t="shared" si="2"/>
+      <c r="V25" s="118">
+        <f t="shared" si="4"/>
         <v>3552.8549500000004</v>
       </c>
-      <c r="W25" s="100" t="str">
-        <f t="shared" si="3"/>
-        <v>Oui</v>
-      </c>
-      <c r="X25" s="177" cm="1">
+      <c r="W25" s="99" t="str">
+        <f t="shared" si="5"/>
+        <v>Oui</v>
+      </c>
+      <c r="X25" s="118" cm="1">
         <f t="array" ref="X25">_xlfn.IFS(W25="Oui",((N25-I25)*0.1),W25="Non",0)</f>
         <v>481.38899999999995</v>
       </c>
-      <c r="Y25" s="100" t="str">
-        <f t="shared" si="4"/>
-        <v>Non</v>
-      </c>
-      <c r="Z25" s="177" cm="1">
+      <c r="Y25" s="99" t="str">
+        <f t="shared" si="6"/>
+        <v>Non</v>
+      </c>
+      <c r="Z25" s="118" cm="1">
         <f t="array" ref="Z25">_xlfn.IFS(Y25="Oui",((O25-J25)*0.1),Y25="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AA25" s="100" t="str">
-        <f t="shared" si="5"/>
-        <v>Non</v>
-      </c>
-      <c r="AB25" s="177" cm="1">
+      <c r="AA25" s="99" t="str">
+        <f t="shared" si="7"/>
+        <v>Non</v>
+      </c>
+      <c r="AB25" s="118" cm="1">
         <f t="array" ref="AB25">_xlfn.IFS(AA25&gt;="Oui",(N25+O25)*0.0025,AA25="Non",0)</f>
         <v>0</v>
       </c>
-      <c r="AC25" s="100" t="str">
-        <f t="shared" si="6"/>
+      <c r="AC25" s="99" t="str">
+        <f t="shared" si="8"/>
+        <v>Non</v>
+      </c>
+      <c r="AD25" s="85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE25" s="85" t="str">
+        <f>IF(AND(P25&gt;=6)*OR('Données brutes'!W25="Oui",'Données brutes'!Y25="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="4.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I26" s="101"/>
-      <c r="J26" s="101"/>
-      <c r="N26" s="178"/>
-      <c r="O26" s="178"/>
-      <c r="V26" s="118"/>
-      <c r="X26" s="118"/>
-      <c r="AB26" s="177"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="119"/>
+      <c r="V26" s="117"/>
+      <c r="X26" s="117"/>
+      <c r="AB26" s="118"/>
     </row>
     <row r="27" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I27" s="179">
-        <f>SUM(I10:I26)</f>
-        <v>1421706.2700000003</v>
-      </c>
-      <c r="J27" s="180">
-        <f>SUM(J10:J26)</f>
-        <v>2521227.1800000002</v>
-      </c>
-      <c r="M27" s="109"/>
-      <c r="N27" s="178">
+      <c r="I27" s="120">
+        <f>SUM(I9:I25)</f>
+        <v>1508346.0400000003</v>
+      </c>
+      <c r="J27" s="121">
+        <f>SUM(J9:J25)</f>
+        <v>2659832.84</v>
+      </c>
+      <c r="M27" s="108"/>
+      <c r="N27" s="119">
         <f>SUM(N9:N25)</f>
         <v>1486480.73</v>
       </c>
-      <c r="O27" s="178">
+      <c r="O27" s="119">
         <f>SUM(O9:O25)</f>
         <v>2596154.92</v>
       </c>
-      <c r="P27" s="108"/>
-      <c r="R27" s="181">
+      <c r="P27" s="107"/>
+      <c r="R27" s="122">
         <f>SUM(R9:R25)</f>
         <v>832655.625</v>
       </c>
-      <c r="S27" s="182">
+      <c r="S27" s="123">
         <f>SUM(S9:S25)</f>
         <v>67960.128899999996</v>
       </c>
-      <c r="V27" s="183">
+      <c r="V27" s="124">
         <f>SUM(V9:V25)</f>
         <v>53807.131099999991</v>
       </c>
-      <c r="X27" s="183">
+      <c r="X27" s="124">
         <f>SUM(X9:X25)</f>
         <v>4659.7329999999974</v>
       </c>
-      <c r="Y27" s="108"/>
-      <c r="Z27" s="183">
+      <c r="Y27" s="107"/>
+      <c r="Z27" s="124">
         <f>SUM(Z9:Z25)</f>
         <v>9516.9704999999994</v>
       </c>
-      <c r="AA27" s="111"/>
-      <c r="AB27" s="177">
+      <c r="AA27" s="110"/>
+      <c r="AB27" s="118">
         <f>SUM(AB9:AB25)</f>
         <v>5241.0172250000005</v>
       </c>
-      <c r="AC27" s="108"/>
-      <c r="AD27" s="112"/>
-      <c r="AE27" s="108"/>
-      <c r="AF27" s="112"/>
-      <c r="AG27" s="110"/>
-      <c r="AH27" s="110"/>
-      <c r="AI27" s="108"/>
+      <c r="AC27" s="107"/>
+      <c r="AD27" s="111"/>
+      <c r="AE27" s="107"/>
+      <c r="AF27" s="111"/>
+      <c r="AG27" s="109"/>
+      <c r="AH27" s="109"/>
+      <c r="AI27" s="107"/>
     </row>
     <row r="28" spans="1:35" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B29" s="149" t="s">
+      <c r="B29" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="150"/>
-      <c r="D29" s="150"/>
-      <c r="E29" s="149" t="s">
+      <c r="C29" s="175"/>
+      <c r="D29" s="175"/>
+      <c r="E29" s="174" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="151"/>
-      <c r="G29" s="149" t="s">
+      <c r="F29" s="176"/>
+      <c r="G29" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="150"/>
-      <c r="I29" s="150"/>
-      <c r="J29" s="150"/>
-      <c r="K29" s="150"/>
-      <c r="L29" s="150"/>
-      <c r="M29" s="150"/>
-      <c r="N29" s="150"/>
-      <c r="O29" s="150"/>
-      <c r="P29" s="151"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="149" t="s">
+      <c r="H29" s="175"/>
+      <c r="I29" s="175"/>
+      <c r="J29" s="175"/>
+      <c r="K29" s="175"/>
+      <c r="L29" s="175"/>
+      <c r="M29" s="175"/>
+      <c r="N29" s="175"/>
+      <c r="O29" s="175"/>
+      <c r="P29" s="176"/>
+      <c r="Q29" s="106"/>
+      <c r="R29" s="174" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="150"/>
-      <c r="T29" s="150"/>
-      <c r="U29" s="150"/>
-      <c r="V29" s="150"/>
-      <c r="W29" s="150"/>
-      <c r="X29" s="150"/>
-      <c r="Y29" s="150"/>
-      <c r="Z29" s="150"/>
-      <c r="AA29" s="150"/>
-      <c r="AB29" s="150"/>
-      <c r="AC29" s="150"/>
-      <c r="AD29" s="150"/>
-      <c r="AE29" s="150"/>
-      <c r="AF29" s="150"/>
-      <c r="AG29" s="150"/>
-      <c r="AH29" s="151"/>
+      <c r="S29" s="175"/>
+      <c r="T29" s="175"/>
+      <c r="U29" s="175"/>
+      <c r="V29" s="175"/>
+      <c r="W29" s="175"/>
+      <c r="X29" s="175"/>
+      <c r="Y29" s="175"/>
+      <c r="Z29" s="175"/>
+      <c r="AA29" s="175"/>
+      <c r="AB29" s="175"/>
+      <c r="AC29" s="175"/>
+      <c r="AD29" s="175"/>
+      <c r="AE29" s="175"/>
+      <c r="AF29" s="175"/>
+      <c r="AG29" s="175"/>
+      <c r="AH29" s="176"/>
     </row>
     <row r="30" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:35" ht="10.199999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="184">
+        <v>41274</v>
+      </c>
+    </row>
     <row r="32" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V32" s="86"/>
     </row>
     <row r="33" spans="2:2" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="99"/>
+      <c r="B33" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:P29"/>
+    <mergeCell ref="R29:AH29"/>
+    <mergeCell ref="P7:P8"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="L5:P5"/>
     <mergeCell ref="R5:AH5"/>
@@ -7108,14 +7386,6 @@
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="W7:X7"/>
     <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:P29"/>
-    <mergeCell ref="R29:AH29"/>
-    <mergeCell ref="P7:P8"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:J25">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -7124,6 +7394,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E9" unlockedFormula="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7148,15 +7421,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="13.8" x14ac:dyDescent="0.2">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="179" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="174" t="s">
+      <c r="C4" s="180" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="81" t="s">
@@ -7164,25 +7437,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="175"/>
+      <c r="C5" s="181"/>
       <c r="D5" s="63" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="175"/>
+      <c r="C6" s="181"/>
       <c r="D6" s="64" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="175"/>
+      <c r="C7" s="181"/>
       <c r="D7" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="176"/>
+      <c r="C8" s="182"/>
       <c r="D8" s="82" t="s">
         <v>56</v>
       </c>
@@ -7202,7 +7475,7 @@
       <c r="C11" s="65"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="174" t="s">
+      <c r="C12" s="180" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="81" t="s">
@@ -7210,43 +7483,43 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="175"/>
+      <c r="C13" s="181"/>
       <c r="D13" s="63" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="175"/>
+      <c r="C14" s="181"/>
       <c r="D14" s="61" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="175"/>
+      <c r="C15" s="181"/>
       <c r="D15" s="80" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="175"/>
+      <c r="C16" s="181"/>
       <c r="D16" s="61" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="175"/>
+      <c r="C17" s="181"/>
       <c r="D17" s="80" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="175"/>
+      <c r="C18" s="181"/>
       <c r="D18" s="61" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="176"/>
+      <c r="C19" s="182"/>
       <c r="D19" s="82" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Notes de cours et excel
</commit_message>
<xml_diff>
--- a/Excel_Exercice04_OperateursFonctionsCond.xlsx
+++ b/Excel_Exercice04_OperateursFonctionsCond.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilio\OneDrive\Bureau\École\Programmation\Outils et gestion\Remise-C13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F268B76-BBF0-4705-9BAB-03140CEE3F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EBBA0D-763F-4E0A-B318-90A0D123EA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -323,7 +323,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1585,7 +1585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -2046,6 +2046,25 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
@@ -2277,21 +2296,6 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2651,7 +2655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="U1" zoomScale="112" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="U1" zoomScale="96" workbookViewId="0">
       <selection activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
@@ -2679,41 +2683,41 @@
   <sheetData>
     <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:34" ht="19.2" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="125"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="125"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="125"/>
-      <c r="Y2" s="125"/>
-      <c r="Z2" s="125"/>
-      <c r="AA2" s="125"/>
-      <c r="AB2" s="125"/>
-      <c r="AC2" s="125"/>
-      <c r="AD2" s="125"/>
-      <c r="AE2" s="125"/>
-      <c r="AF2" s="125"/>
-      <c r="AG2" s="125"/>
-      <c r="AH2" s="125"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
+      <c r="L2" s="130"/>
+      <c r="M2" s="130"/>
+      <c r="N2" s="130"/>
+      <c r="O2" s="130"/>
+      <c r="P2" s="130"/>
+      <c r="Q2" s="130"/>
+      <c r="R2" s="130"/>
+      <c r="S2" s="130"/>
+      <c r="T2" s="130"/>
+      <c r="U2" s="130"/>
+      <c r="V2" s="130"/>
+      <c r="W2" s="130"/>
+      <c r="X2" s="130"/>
+      <c r="Y2" s="130"/>
+      <c r="Z2" s="130"/>
+      <c r="AA2" s="130"/>
+      <c r="AB2" s="130"/>
+      <c r="AC2" s="130"/>
+      <c r="AD2" s="130"/>
+      <c r="AE2" s="130"/>
+      <c r="AF2" s="130"/>
+      <c r="AG2" s="130"/>
+      <c r="AH2" s="130"/>
     </row>
     <row r="3" spans="2:34" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -2724,122 +2728,122 @@
     </row>
     <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
-      <c r="L5" s="127" t="s">
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="L5" s="132" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="127"/>
-      <c r="N5" s="127"/>
-      <c r="O5" s="127"/>
-      <c r="P5" s="127"/>
-      <c r="R5" s="131" t="s">
+      <c r="M5" s="132"/>
+      <c r="N5" s="132"/>
+      <c r="O5" s="132"/>
+      <c r="P5" s="132"/>
+      <c r="R5" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="131"/>
-      <c r="T5" s="131"/>
-      <c r="U5" s="131"/>
-      <c r="V5" s="131"/>
-      <c r="W5" s="131"/>
-      <c r="X5" s="131"/>
-      <c r="Y5" s="131"/>
-      <c r="Z5" s="131"/>
-      <c r="AA5" s="131"/>
-      <c r="AB5" s="131"/>
-      <c r="AC5" s="131"/>
-      <c r="AD5" s="131"/>
-      <c r="AE5" s="131"/>
-      <c r="AF5" s="131"/>
-      <c r="AG5" s="131"/>
-      <c r="AH5" s="131"/>
+      <c r="S5" s="136"/>
+      <c r="T5" s="136"/>
+      <c r="U5" s="136"/>
+      <c r="V5" s="136"/>
+      <c r="W5" s="136"/>
+      <c r="X5" s="136"/>
+      <c r="Y5" s="136"/>
+      <c r="Z5" s="136"/>
+      <c r="AA5" s="136"/>
+      <c r="AB5" s="136"/>
+      <c r="AC5" s="136"/>
+      <c r="AD5" s="136"/>
+      <c r="AE5" s="136"/>
+      <c r="AF5" s="136"/>
+      <c r="AG5" s="136"/>
+      <c r="AH5" s="136"/>
     </row>
     <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="153" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="140" t="s">
+      <c r="C7" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="142" t="s">
+      <c r="D7" s="147" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="144" t="s">
+      <c r="F7" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="134" t="s">
+      <c r="G7" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="135"/>
-      <c r="I7" s="146" t="s">
+      <c r="H7" s="140"/>
+      <c r="I7" s="151" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="147"/>
+      <c r="J7" s="152"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="136" t="s">
+      <c r="L7" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="137"/>
-      <c r="N7" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="137"/>
-      <c r="P7" s="150" t="s">
+      <c r="M7" s="142"/>
+      <c r="N7" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="142"/>
+      <c r="P7" s="155" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="138" t="s">
+      <c r="R7" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="139"/>
+      <c r="S7" s="144"/>
       <c r="T7" s="11"/>
-      <c r="U7" s="138" t="s">
+      <c r="U7" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="139"/>
-      <c r="W7" s="138" t="s">
+      <c r="V7" s="144"/>
+      <c r="W7" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="139"/>
-      <c r="Y7" s="138" t="s">
+      <c r="X7" s="144"/>
+      <c r="Y7" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="139"/>
-      <c r="AA7" s="138" t="s">
+      <c r="Z7" s="144"/>
+      <c r="AA7" s="143" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="139"/>
-      <c r="AC7" s="138" t="s">
+      <c r="AB7" s="144"/>
+      <c r="AC7" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="139"/>
-      <c r="AE7" s="138" t="s">
+      <c r="AD7" s="144"/>
+      <c r="AE7" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="139"/>
+      <c r="AF7" s="144"/>
       <c r="AG7" s="11"/>
-      <c r="AH7" s="152" t="s">
+      <c r="AH7" s="157" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="149"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="143"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="145"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="148"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="150"/>
       <c r="G8" s="13" t="s">
         <v>9</v>
       </c>
@@ -2865,7 +2869,7 @@
       <c r="O8" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="151"/>
+      <c r="P8" s="156"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="20" t="s">
         <v>9</v>
@@ -2911,7 +2915,7 @@
         <v>40</v>
       </c>
       <c r="AG8" s="12"/>
-      <c r="AH8" s="153"/>
+      <c r="AH8" s="158"/>
     </row>
     <row r="9" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="37" t="s">
@@ -4915,46 +4919,46 @@
       <c r="AH28" s="4"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B29" s="128" t="s">
+      <c r="B29" s="133" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="129"/>
-      <c r="D29" s="130"/>
-      <c r="E29" s="128" t="s">
+      <c r="C29" s="134"/>
+      <c r="D29" s="135"/>
+      <c r="E29" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="130"/>
-      <c r="G29" s="128" t="s">
+      <c r="F29" s="135"/>
+      <c r="G29" s="133" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="129"/>
-      <c r="I29" s="129"/>
-      <c r="J29" s="129"/>
-      <c r="K29" s="129"/>
-      <c r="L29" s="129"/>
-      <c r="M29" s="129"/>
-      <c r="N29" s="129"/>
-      <c r="O29" s="129"/>
-      <c r="P29" s="130"/>
-      <c r="R29" s="128" t="s">
+      <c r="H29" s="134"/>
+      <c r="I29" s="134"/>
+      <c r="J29" s="134"/>
+      <c r="K29" s="134"/>
+      <c r="L29" s="134"/>
+      <c r="M29" s="134"/>
+      <c r="N29" s="134"/>
+      <c r="O29" s="134"/>
+      <c r="P29" s="135"/>
+      <c r="R29" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="129"/>
-      <c r="T29" s="129"/>
-      <c r="U29" s="129"/>
-      <c r="V29" s="129"/>
-      <c r="W29" s="129"/>
-      <c r="X29" s="129"/>
-      <c r="Y29" s="129"/>
-      <c r="Z29" s="129"/>
-      <c r="AA29" s="129"/>
-      <c r="AB29" s="129"/>
-      <c r="AC29" s="129"/>
-      <c r="AD29" s="129"/>
-      <c r="AE29" s="129"/>
-      <c r="AF29" s="129"/>
-      <c r="AG29" s="129"/>
-      <c r="AH29" s="130"/>
+      <c r="S29" s="134"/>
+      <c r="T29" s="134"/>
+      <c r="U29" s="134"/>
+      <c r="V29" s="134"/>
+      <c r="W29" s="134"/>
+      <c r="X29" s="134"/>
+      <c r="Y29" s="134"/>
+      <c r="Z29" s="134"/>
+      <c r="AA29" s="134"/>
+      <c r="AB29" s="134"/>
+      <c r="AC29" s="134"/>
+      <c r="AD29" s="134"/>
+      <c r="AE29" s="134"/>
+      <c r="AF29" s="134"/>
+      <c r="AG29" s="134"/>
+      <c r="AH29" s="135"/>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="E31" s="8"/>
@@ -5307,8 +5311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="AI8" sqref="AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -5385,110 +5389,110 @@
       <c r="C4" s="105"/>
     </row>
     <row r="5" spans="1:34" ht="16.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="154" t="s">
+      <c r="B5" s="159" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="155"/>
-      <c r="H5" s="155"/>
-      <c r="I5" s="155"/>
-      <c r="J5" s="155"/>
-      <c r="L5" s="156" t="s">
+      <c r="C5" s="160"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="160"/>
+      <c r="L5" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="157"/>
-      <c r="N5" s="157"/>
-      <c r="O5" s="157"/>
-      <c r="P5" s="157"/>
-      <c r="R5" s="158" t="s">
+      <c r="M5" s="162"/>
+      <c r="N5" s="162"/>
+      <c r="O5" s="162"/>
+      <c r="P5" s="162"/>
+      <c r="R5" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="159"/>
-      <c r="T5" s="159"/>
-      <c r="U5" s="159"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
-      <c r="X5" s="159"/>
-      <c r="Y5" s="159"/>
-      <c r="Z5" s="159"/>
-      <c r="AA5" s="159"/>
-      <c r="AB5" s="159"/>
-      <c r="AC5" s="159"/>
-      <c r="AD5" s="159"/>
-      <c r="AE5" s="159"/>
-      <c r="AF5" s="159"/>
-      <c r="AG5" s="159"/>
-      <c r="AH5" s="159"/>
+      <c r="S5" s="164"/>
+      <c r="T5" s="164"/>
+      <c r="U5" s="164"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
+      <c r="X5" s="164"/>
+      <c r="Y5" s="164"/>
+      <c r="Z5" s="164"/>
+      <c r="AA5" s="164"/>
+      <c r="AB5" s="164"/>
+      <c r="AC5" s="164"/>
+      <c r="AD5" s="164"/>
+      <c r="AE5" s="164"/>
+      <c r="AF5" s="164"/>
+      <c r="AG5" s="164"/>
+      <c r="AH5" s="164"/>
     </row>
     <row r="6" spans="1:34" s="101" customFormat="1" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="87"/>
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="167" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="162" t="s">
+      <c r="C7" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="164" t="s">
+      <c r="D7" s="169" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="166" t="s">
+      <c r="E7" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="168" t="s">
+      <c r="F7" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="160" t="s">
+      <c r="G7" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="161"/>
-      <c r="I7" s="170" t="s">
+      <c r="H7" s="166"/>
+      <c r="I7" s="175" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="171"/>
-      <c r="L7" s="172" t="s">
+      <c r="J7" s="176"/>
+      <c r="L7" s="177" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="172"/>
-      <c r="N7" s="172" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="172"/>
-      <c r="P7" s="177" t="s">
+      <c r="M7" s="177"/>
+      <c r="N7" s="177" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="177"/>
+      <c r="P7" s="182" t="s">
         <v>42</v>
       </c>
-      <c r="R7" s="173" t="s">
+      <c r="R7" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="173"/>
+      <c r="S7" s="178"/>
       <c r="T7" s="115"/>
-      <c r="U7" s="173" t="s">
+      <c r="U7" s="178" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="173"/>
-      <c r="W7" s="173" t="s">
+      <c r="V7" s="178"/>
+      <c r="W7" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="173"/>
-      <c r="Y7" s="173" t="s">
+      <c r="X7" s="178"/>
+      <c r="Y7" s="178" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="173"/>
-      <c r="AA7" s="173" t="s">
+      <c r="Z7" s="178"/>
+      <c r="AA7" s="178" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="173"/>
-      <c r="AC7" s="173" t="s">
+      <c r="AB7" s="178"/>
+      <c r="AC7" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="173"/>
-      <c r="AE7" s="173" t="s">
+      <c r="AD7" s="178"/>
+      <c r="AE7" s="178" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="173"/>
+      <c r="AF7" s="178"/>
       <c r="AG7" s="115"/>
       <c r="AH7" s="116" t="s">
         <v>50</v>
@@ -5496,11 +5500,11 @@
     </row>
     <row r="8" spans="1:34" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="87"/>
-      <c r="B8" s="163"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="167"/>
-      <c r="F8" s="169"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="174"/>
       <c r="G8" s="95" t="s">
         <v>9</v>
       </c>
@@ -5525,7 +5529,7 @@
       <c r="O8" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="178"/>
+      <c r="P8" s="183"/>
       <c r="R8" s="112" t="s">
         <v>9</v>
       </c>
@@ -5583,11 +5587,11 @@
       <c r="D9" s="92">
         <v>38226</v>
       </c>
-      <c r="E9" s="183">
+      <c r="E9" s="125">
         <f>YEARFRAC(D9,$B$31)</f>
         <v>8.344444444444445</v>
       </c>
-      <c r="F9" s="186">
+      <c r="F9" s="128">
         <f>IF(MOD(E9,5) &gt;=0,ROUNDDOWN(E9/5+2,0),0)</f>
         <v>3</v>
       </c>
@@ -5603,10 +5607,10 @@
       <c r="J9" s="94">
         <v>138605.66</v>
       </c>
-      <c r="L9" s="185">
+      <c r="L9" s="127">
         <v>1837.5</v>
       </c>
-      <c r="M9" s="185">
+      <c r="M9" s="127">
         <v>12.7</v>
       </c>
       <c r="N9" s="119">
@@ -5661,15 +5665,15 @@
         <f>IF(AND(Y9="Oui",W9="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
-      <c r="AD9" s="85">
-        <f>IF(AND(W9="Oui",Y9="Oui"),(O9-J9)+(N9-I9)*(P9/100),0)</f>
-        <v>0</v>
+      <c r="AD9" s="129" cm="1">
+        <f t="array" ref="AD9">_xlfn.IFS(W9="Oui",((J9-O9)+(I9-N9)*(P9/100)),(AND(W9="Oui",Y9="Oui")),0)</f>
+        <v>25048.916400000002</v>
       </c>
       <c r="AE9" s="85" t="str">
         <f>IF(AND(P9&gt;=6)*OR('Données brutes'!W9="Oui",'Données brutes'!Y9="Oui"),"Oui","Non")</f>
         <v>Oui</v>
       </c>
-      <c r="AF9" s="85">
+      <c r="AF9" s="129">
         <f>IF(AE9="Oui",(15000/8)/(N9/O9),0)</f>
         <v>2440.2661331289892</v>
       </c>
@@ -5685,11 +5689,11 @@
       <c r="D10" s="92">
         <v>37601</v>
       </c>
-      <c r="E10" s="183">
+      <c r="E10" s="125">
         <f t="shared" ref="E10:E25" si="0">YEARFRAC(D10,$B$31)</f>
         <v>10.055555555555555</v>
       </c>
-      <c r="F10" s="185">
+      <c r="F10" s="127">
         <f t="shared" ref="F10:F25" si="1">IF(MOD(E10,5) &gt;=0,ROUNDDOWN(E10/5+2,0),0)</f>
         <v>4</v>
       </c>
@@ -5705,10 +5709,10 @@
       <c r="J10" s="94">
         <v>141119.44</v>
       </c>
-      <c r="L10" s="185">
+      <c r="L10" s="127">
         <v>1800</v>
       </c>
-      <c r="M10" s="185">
+      <c r="M10" s="127">
         <v>25.2</v>
       </c>
       <c r="N10" s="119">
@@ -5763,13 +5767,17 @@
         <f t="shared" ref="AC10:AC25" si="8">IF(AND(Y10="Oui",W10="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
-      <c r="AD10" s="85">
-        <f t="shared" ref="AD10:AD25" si="9">IF(AND(W10="Oui",Y10="Oui"),(O10-J10)+(N10-I10)*(P10/100),0)</f>
-        <v>0</v>
+      <c r="AD10" s="129" cm="1">
+        <f t="array" ref="AD10">_xlfn.IFS(W10="Oui",((J10-O10)+(I10-N10)*(P10/100)),(AND(W10="Oui",Y10="Oui")),0)</f>
+        <v>7628.9304000000102</v>
       </c>
       <c r="AE10" s="85" t="str">
         <f>IF(AND(P10&gt;=6)*OR('Données brutes'!W10="Oui",'Données brutes'!Y10="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF10" s="129">
+        <f t="shared" ref="AF10:AF25" si="9">IF(AE10="Oui",(15000/8)/(N10/O10),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5783,11 +5791,11 @@
       <c r="D11" s="92">
         <v>35826</v>
       </c>
-      <c r="E11" s="183">
+      <c r="E11" s="125">
         <f t="shared" si="0"/>
         <v>14.916666666666666</v>
       </c>
-      <c r="F11" s="185">
+      <c r="F11" s="127">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -5803,10 +5811,10 @@
       <c r="J11" s="94">
         <v>156292.04</v>
       </c>
-      <c r="L11" s="185">
+      <c r="L11" s="127">
         <v>1800</v>
       </c>
-      <c r="M11" s="185">
+      <c r="M11" s="127">
         <v>0</v>
       </c>
       <c r="N11" s="119">
@@ -5861,13 +5869,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD11" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD11" s="129" t="e" cm="1">
+        <f t="array" ref="AD11">_xlfn.IFS(W11="Oui",((J11-O11)+(I11-N11)*(P11/100)),(AND(W11="Oui",Y11="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE11" s="85" t="str">
         <f>IF(AND(P11&gt;=6)*OR('Données brutes'!W11="Oui",'Données brutes'!Y11="Oui"),"Oui","Non")</f>
         <v>Oui</v>
+      </c>
+      <c r="AF11" s="129">
+        <f t="shared" si="9"/>
+        <v>3874.0759129866442</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5881,11 +5893,11 @@
       <c r="D12" s="92">
         <v>35403</v>
       </c>
-      <c r="E12" s="183">
+      <c r="E12" s="125">
         <f t="shared" si="0"/>
         <v>16.074999999999999</v>
       </c>
-      <c r="F12" s="185">
+      <c r="F12" s="127">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -5901,10 +5913,10 @@
       <c r="J12" s="94">
         <v>156576.41</v>
       </c>
-      <c r="L12" s="185">
+      <c r="L12" s="127">
         <v>1762.5</v>
       </c>
-      <c r="M12" s="185">
+      <c r="M12" s="127">
         <v>0</v>
       </c>
       <c r="N12" s="119">
@@ -5959,13 +5971,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD12" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD12" s="129" t="e" cm="1">
+        <f t="array" ref="AD12">_xlfn.IFS(W12="Oui",((J12-O12)+(I12-N12)*(P12/100)),(AND(W12="Oui",Y12="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE12" s="85" t="str">
         <f>IF(AND(P12&gt;=6)*OR('Données brutes'!W12="Oui",'Données brutes'!Y12="Oui"),"Oui","Non")</f>
         <v>Oui</v>
+      </c>
+      <c r="AF12" s="129">
+        <f t="shared" si="9"/>
+        <v>4110.2243420618061</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5979,11 +5995,11 @@
       <c r="D13" s="92">
         <v>33093</v>
       </c>
-      <c r="E13" s="183">
+      <c r="E13" s="125">
         <f t="shared" si="0"/>
         <v>22.397222222222222</v>
       </c>
-      <c r="F13" s="185">
+      <c r="F13" s="127">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -5999,10 +6015,10 @@
       <c r="J13" s="94">
         <v>172168.01</v>
       </c>
-      <c r="L13" s="185">
+      <c r="L13" s="127">
         <v>1725</v>
       </c>
-      <c r="M13" s="185">
+      <c r="M13" s="127">
         <v>39.57</v>
       </c>
       <c r="N13" s="119">
@@ -6057,13 +6073,17 @@
         <f t="shared" si="8"/>
         <v>Oui</v>
       </c>
-      <c r="AD13" s="85">
-        <f t="shared" si="9"/>
-        <v>5705.6844999999948</v>
+      <c r="AD13" s="129" cm="1">
+        <f t="array" ref="AD13">_xlfn.IFS(W13="Oui",((J13-O13)+(I13-N13)*(P13/100)),(AND(W13="Oui",Y13="Oui")),0)</f>
+        <v>-5705.6844999999948</v>
       </c>
       <c r="AE13" s="85" t="str">
         <f>IF(AND(P13&gt;=6)*OR('Données brutes'!W13="Oui",'Données brutes'!Y13="Oui"),"Oui","Non")</f>
         <v>Oui</v>
+      </c>
+      <c r="AF13" s="129">
+        <f t="shared" si="9"/>
+        <v>3458.4834155824237</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6077,11 +6097,11 @@
       <c r="D14" s="92">
         <v>37900</v>
       </c>
-      <c r="E14" s="183">
+      <c r="E14" s="125">
         <f t="shared" si="0"/>
         <v>9.2361111111111107</v>
       </c>
-      <c r="F14" s="185">
+      <c r="F14" s="127">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -6097,10 +6117,10 @@
       <c r="J14" s="94">
         <v>141450.34</v>
       </c>
-      <c r="L14" s="185">
+      <c r="L14" s="127">
         <v>1837.5</v>
       </c>
-      <c r="M14" s="185">
+      <c r="M14" s="127">
         <v>98.2</v>
       </c>
       <c r="N14" s="119">
@@ -6155,13 +6175,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD14" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD14" s="129" t="e" cm="1">
+        <f t="array" ref="AD14">_xlfn.IFS(W14="Oui",((J14-O14)+(I14-N14)*(P14/100)),(AND(W14="Oui",Y14="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE14" s="85" t="str">
         <f>IF(AND(P14&gt;=6)*OR('Données brutes'!W14="Oui",'Données brutes'!Y14="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF14" s="129">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6175,11 +6199,11 @@
       <c r="D15" s="92">
         <v>35590</v>
       </c>
-      <c r="E15" s="183">
+      <c r="E15" s="125">
         <f t="shared" si="0"/>
         <v>15.561111111111112</v>
       </c>
-      <c r="F15" s="185">
+      <c r="F15" s="127">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -6195,10 +6219,10 @@
       <c r="J15" s="94">
         <v>155011.24</v>
       </c>
-      <c r="L15" s="185">
+      <c r="L15" s="127">
         <v>1762.5</v>
       </c>
-      <c r="M15" s="185">
+      <c r="M15" s="127">
         <v>244.14</v>
       </c>
       <c r="N15" s="119">
@@ -6253,13 +6277,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD15" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD15" s="129" cm="1">
+        <f t="array" ref="AD15">_xlfn.IFS(W15="Oui",((J15-O15)+(I15-N15)*(P15/100)),(AND(W15="Oui",Y15="Oui")),0)</f>
+        <v>34852.488199999993</v>
       </c>
       <c r="AE15" s="85" t="str">
         <f>IF(AND(P15&gt;=6)*OR('Données brutes'!W15="Oui",'Données brutes'!Y15="Oui"),"Oui","Non")</f>
         <v>Oui</v>
+      </c>
+      <c r="AF15" s="129">
+        <f t="shared" si="9"/>
+        <v>2267.9655535239849</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6273,11 +6301,11 @@
       <c r="D16" s="92">
         <v>35192</v>
       </c>
-      <c r="E16" s="183">
+      <c r="E16" s="125">
         <f t="shared" si="0"/>
         <v>16.649999999999999</v>
       </c>
-      <c r="F16" s="185">
+      <c r="F16" s="127">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -6293,10 +6321,10 @@
       <c r="J16" s="94">
         <v>158342.45000000001</v>
       </c>
-      <c r="L16" s="185">
+      <c r="L16" s="127">
         <v>1762.5</v>
       </c>
-      <c r="M16" s="185">
+      <c r="M16" s="127">
         <v>109.39</v>
       </c>
       <c r="N16" s="119">
@@ -6351,13 +6379,17 @@
         <f t="shared" si="8"/>
         <v>Oui</v>
       </c>
-      <c r="AD16" s="85">
-        <f t="shared" si="9"/>
-        <v>6544.3416000000007</v>
+      <c r="AD16" s="129" cm="1">
+        <f t="array" ref="AD16">_xlfn.IFS(W16="Oui",((J16-O16)+(I16-N16)*(P16/100)),(AND(W16="Oui",Y16="Oui")),0)</f>
+        <v>-6544.3416000000007</v>
       </c>
       <c r="AE16" s="85" t="str">
         <f>IF(AND(P16&gt;=6)*OR('Données brutes'!W16="Oui",'Données brutes'!Y16="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF16" s="129">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6371,11 +6403,11 @@
       <c r="D17" s="92">
         <v>36628</v>
       </c>
-      <c r="E17" s="183">
+      <c r="E17" s="125">
         <f t="shared" si="0"/>
         <v>12.719444444444445</v>
       </c>
-      <c r="F17" s="185">
+      <c r="F17" s="127">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -6391,10 +6423,10 @@
       <c r="J17" s="94">
         <v>149436.59</v>
       </c>
-      <c r="L17" s="185">
+      <c r="L17" s="127">
         <v>1800</v>
       </c>
-      <c r="M17" s="185">
+      <c r="M17" s="127">
         <v>0</v>
       </c>
       <c r="N17" s="119">
@@ -6449,13 +6481,17 @@
         <f t="shared" si="8"/>
         <v>Oui</v>
       </c>
-      <c r="AD17" s="85">
-        <f t="shared" si="9"/>
-        <v>743.67140000000506</v>
+      <c r="AD17" s="129" cm="1">
+        <f t="array" ref="AD17">_xlfn.IFS(W17="Oui",((J17-O17)+(I17-N17)*(P17/100)),(AND(W17="Oui",Y17="Oui")),0)</f>
+        <v>-743.67140000000506</v>
       </c>
       <c r="AE17" s="85" t="str">
         <f>IF(AND(P17&gt;=6)*OR('Données brutes'!W17="Oui",'Données brutes'!Y17="Oui"),"Oui","Non")</f>
         <v>Oui</v>
+      </c>
+      <c r="AF17" s="129">
+        <f t="shared" si="9"/>
+        <v>3032.0045480120184</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6469,11 +6505,11 @@
       <c r="D18" s="92">
         <v>30115</v>
       </c>
-      <c r="E18" s="183">
+      <c r="E18" s="125">
         <f t="shared" si="0"/>
         <v>30.55</v>
       </c>
-      <c r="F18" s="185">
+      <c r="F18" s="127">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -6489,10 +6525,10 @@
       <c r="J18" s="94">
         <v>188016.91</v>
       </c>
-      <c r="L18" s="185">
+      <c r="L18" s="127">
         <v>1650</v>
       </c>
-      <c r="M18" s="185">
+      <c r="M18" s="127">
         <v>143.27000000000001</v>
       </c>
       <c r="N18" s="119">
@@ -6547,13 +6583,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD18" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD18" s="129" t="e" cm="1">
+        <f t="array" ref="AD18">_xlfn.IFS(W18="Oui",((J18-O18)+(I18-N18)*(P18/100)),(AND(W18="Oui",Y18="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE18" s="85" t="str">
         <f>IF(AND(P18&gt;=6)*OR('Données brutes'!W18="Oui",'Données brutes'!Y18="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF18" s="129">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6567,11 +6607,11 @@
       <c r="D19" s="92">
         <v>41231</v>
       </c>
-      <c r="E19" s="183">
+      <c r="E19" s="125">
         <f t="shared" si="0"/>
         <v>0.11944444444444445</v>
       </c>
-      <c r="F19" s="185">
+      <c r="F19" s="127">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -6587,10 +6627,10 @@
       <c r="J19" s="94">
         <v>114677.5</v>
       </c>
-      <c r="L19" s="185">
+      <c r="L19" s="127">
         <v>1875</v>
       </c>
-      <c r="M19" s="185">
+      <c r="M19" s="127">
         <v>0</v>
       </c>
       <c r="N19" s="119">
@@ -6645,13 +6685,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD19" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD19" s="129" t="e" cm="1">
+        <f t="array" ref="AD19">_xlfn.IFS(W19="Oui",((J19-O19)+(I19-N19)*(P19/100)),(AND(W19="Oui",Y19="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE19" s="85" t="str">
         <f>IF(AND(P19&gt;=6)*OR('Données brutes'!W19="Oui",'Données brutes'!Y19="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF19" s="129">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6665,11 +6709,11 @@
       <c r="D20" s="92">
         <v>31824</v>
       </c>
-      <c r="E20" s="183">
+      <c r="E20" s="125">
         <f t="shared" si="0"/>
         <v>25.875</v>
       </c>
-      <c r="F20" s="185">
+      <c r="F20" s="127">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -6685,10 +6729,10 @@
       <c r="J20" s="94">
         <v>178594.61</v>
       </c>
-      <c r="L20" s="185">
+      <c r="L20" s="127">
         <v>1687.5</v>
       </c>
-      <c r="M20" s="185">
+      <c r="M20" s="127">
         <v>145.13</v>
       </c>
       <c r="N20" s="119">
@@ -6743,13 +6787,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD20" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD20" s="129" t="e" cm="1">
+        <f t="array" ref="AD20">_xlfn.IFS(W20="Oui",((J20-O20)+(I20-N20)*(P20/100)),(AND(W20="Oui",Y20="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE20" s="85" t="str">
         <f>IF(AND(P20&gt;=6)*OR('Données brutes'!W20="Oui",'Données brutes'!Y20="Oui"),"Oui","Non")</f>
         <v>Oui</v>
+      </c>
+      <c r="AF20" s="129">
+        <f t="shared" si="9"/>
+        <v>3723.7497425452734</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6763,11 +6811,11 @@
       <c r="D21" s="92">
         <v>38150</v>
       </c>
-      <c r="E21" s="183">
+      <c r="E21" s="125">
         <f t="shared" si="0"/>
         <v>8.5527777777777771</v>
       </c>
-      <c r="F21" s="185">
+      <c r="F21" s="127">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -6783,10 +6831,10 @@
       <c r="J21" s="94">
         <v>139268.84</v>
       </c>
-      <c r="L21" s="185">
+      <c r="L21" s="127">
         <v>1837.5</v>
       </c>
-      <c r="M21" s="185">
+      <c r="M21" s="127">
         <v>191.85</v>
       </c>
       <c r="N21" s="119">
@@ -6841,13 +6889,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD21" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD21" s="129" cm="1">
+        <f t="array" ref="AD21">_xlfn.IFS(W21="Oui",((J21-O21)+(I21-N21)*(P21/100)),(AND(W21="Oui",Y21="Oui")),0)</f>
+        <v>-19.860599999997788</v>
       </c>
       <c r="AE21" s="85" t="str">
         <f>IF(AND(P21&gt;=6)*OR('Données brutes'!W21="Oui",'Données brutes'!Y21="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF21" s="129">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6861,11 +6913,11 @@
       <c r="D22" s="92">
         <v>32891</v>
       </c>
-      <c r="E22" s="183">
+      <c r="E22" s="125">
         <f t="shared" si="0"/>
         <v>22.952777777777779</v>
       </c>
-      <c r="F22" s="185">
+      <c r="F22" s="127">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -6881,10 +6933,10 @@
       <c r="J22" s="94">
         <v>173822.75</v>
       </c>
-      <c r="L22" s="185">
+      <c r="L22" s="127">
         <v>1725</v>
       </c>
-      <c r="M22" s="185">
+      <c r="M22" s="127">
         <v>150.72</v>
       </c>
       <c r="N22" s="119">
@@ -6939,13 +6991,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD22" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD22" s="129" t="e" cm="1">
+        <f t="array" ref="AD22">_xlfn.IFS(W22="Oui",((J22-O22)+(I22-N22)*(P22/100)),(AND(W22="Oui",Y22="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE22" s="85" t="str">
         <f>IF(AND(P22&gt;=6)*OR('Données brutes'!W22="Oui",'Données brutes'!Y22="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF22" s="129">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -6959,11 +7015,11 @@
       <c r="D23" s="92">
         <v>41102</v>
       </c>
-      <c r="E23" s="183">
+      <c r="E23" s="125">
         <f t="shared" si="0"/>
         <v>0.46944444444444444</v>
       </c>
-      <c r="F23" s="185">
+      <c r="F23" s="127">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -6979,10 +7035,10 @@
       <c r="J23" s="94">
         <v>115826.13</v>
       </c>
-      <c r="L23" s="185">
+      <c r="L23" s="127">
         <v>1875</v>
       </c>
-      <c r="M23" s="185">
+      <c r="M23" s="127">
         <v>159.16999999999999</v>
       </c>
       <c r="N23" s="119">
@@ -7037,13 +7093,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD23" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD23" s="129" t="e" cm="1">
+        <f t="array" ref="AD23">_xlfn.IFS(W23="Oui",((J23-O23)+(I23-N23)*(P23/100)),(AND(W23="Oui",Y23="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE23" s="85" t="str">
         <f>IF(AND(P23&gt;=6)*OR('Données brutes'!W23="Oui",'Données brutes'!Y23="Oui"),"Oui","Non")</f>
         <v>Oui</v>
+      </c>
+      <c r="AF23" s="129">
+        <f t="shared" si="9"/>
+        <v>3184.353807287579</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -7057,11 +7117,11 @@
       <c r="D24" s="92">
         <v>29465</v>
       </c>
-      <c r="E24" s="183">
+      <c r="E24" s="125">
         <f t="shared" si="0"/>
         <v>32.333333333333336</v>
       </c>
-      <c r="F24" s="185">
+      <c r="F24" s="127">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -7077,10 +7137,10 @@
       <c r="J24" s="94">
         <v>193110.06</v>
       </c>
-      <c r="L24" s="185">
+      <c r="L24" s="127">
         <v>1650</v>
       </c>
-      <c r="M24" s="185">
+      <c r="M24" s="127">
         <v>0</v>
       </c>
       <c r="N24" s="119">
@@ -7135,13 +7195,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD24" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD24" s="129" t="e" cm="1">
+        <f t="array" ref="AD24">_xlfn.IFS(W24="Oui",((J24-O24)+(I24-N24)*(P24/100)),(AND(W24="Oui",Y24="Oui")),0)</f>
+        <v>#N/A</v>
       </c>
       <c r="AE24" s="85" t="str">
         <f>IF(AND(P24&gt;=6)*OR('Données brutes'!W24="Oui",'Données brutes'!Y24="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF24" s="129">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -7155,11 +7219,11 @@
       <c r="D25" s="92">
         <v>30711</v>
       </c>
-      <c r="E25" s="183">
+      <c r="E25" s="125">
         <f t="shared" si="0"/>
         <v>28.916666666666668</v>
       </c>
-      <c r="F25" s="185">
+      <c r="F25" s="127">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -7175,10 +7239,10 @@
       <c r="J25" s="94">
         <v>187513.86</v>
       </c>
-      <c r="L25" s="185">
+      <c r="L25" s="127">
         <v>1687.5</v>
       </c>
-      <c r="M25" s="185">
+      <c r="M25" s="127">
         <v>226.41</v>
       </c>
       <c r="N25" s="119">
@@ -7233,13 +7297,17 @@
         <f t="shared" si="8"/>
         <v>Non</v>
       </c>
-      <c r="AD25" s="85">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="AD25" s="129" cm="1">
+        <f t="array" ref="AD25">_xlfn.IFS(W25="Oui",((J25-O25)+(I25-N25)*(P25/100)),(AND(W25="Oui",Y25="Oui")),0)</f>
+        <v>15935.255499999983</v>
       </c>
       <c r="AE25" s="85" t="str">
         <f>IF(AND(P25&gt;=6)*OR('Données brutes'!W25="Oui",'Données brutes'!Y25="Oui"),"Oui","Non")</f>
         <v>Non</v>
+      </c>
+      <c r="AF25" s="129">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="4.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -7306,51 +7374,51 @@
     </row>
     <row r="28" spans="1:35" ht="4.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B29" s="174" t="s">
+      <c r="B29" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="175"/>
-      <c r="D29" s="175"/>
-      <c r="E29" s="174" t="s">
+      <c r="C29" s="180"/>
+      <c r="D29" s="180"/>
+      <c r="E29" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="176"/>
-      <c r="G29" s="174" t="s">
+      <c r="F29" s="181"/>
+      <c r="G29" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="175"/>
-      <c r="I29" s="175"/>
-      <c r="J29" s="175"/>
-      <c r="K29" s="175"/>
-      <c r="L29" s="175"/>
-      <c r="M29" s="175"/>
-      <c r="N29" s="175"/>
-      <c r="O29" s="175"/>
-      <c r="P29" s="176"/>
+      <c r="H29" s="180"/>
+      <c r="I29" s="180"/>
+      <c r="J29" s="180"/>
+      <c r="K29" s="180"/>
+      <c r="L29" s="180"/>
+      <c r="M29" s="180"/>
+      <c r="N29" s="180"/>
+      <c r="O29" s="180"/>
+      <c r="P29" s="181"/>
       <c r="Q29" s="106"/>
-      <c r="R29" s="174" t="s">
+      <c r="R29" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="175"/>
-      <c r="T29" s="175"/>
-      <c r="U29" s="175"/>
-      <c r="V29" s="175"/>
-      <c r="W29" s="175"/>
-      <c r="X29" s="175"/>
-      <c r="Y29" s="175"/>
-      <c r="Z29" s="175"/>
-      <c r="AA29" s="175"/>
-      <c r="AB29" s="175"/>
-      <c r="AC29" s="175"/>
-      <c r="AD29" s="175"/>
-      <c r="AE29" s="175"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="175"/>
-      <c r="AH29" s="176"/>
+      <c r="S29" s="180"/>
+      <c r="T29" s="180"/>
+      <c r="U29" s="180"/>
+      <c r="V29" s="180"/>
+      <c r="W29" s="180"/>
+      <c r="X29" s="180"/>
+      <c r="Y29" s="180"/>
+      <c r="Z29" s="180"/>
+      <c r="AA29" s="180"/>
+      <c r="AB29" s="180"/>
+      <c r="AC29" s="180"/>
+      <c r="AD29" s="180"/>
+      <c r="AE29" s="180"/>
+      <c r="AF29" s="180"/>
+      <c r="AG29" s="180"/>
+      <c r="AH29" s="181"/>
     </row>
     <row r="30" spans="1:35" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:35" ht="10.199999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="184">
+      <c r="B31" s="126">
         <v>41274</v>
       </c>
     </row>
@@ -7421,15 +7489,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="13.8" x14ac:dyDescent="0.2">
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="184" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="180" t="s">
+      <c r="C4" s="185" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="81" t="s">
@@ -7437,25 +7505,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="181"/>
+      <c r="C5" s="186"/>
       <c r="D5" s="63" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="181"/>
+      <c r="C6" s="186"/>
       <c r="D6" s="64" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="181"/>
+      <c r="C7" s="186"/>
       <c r="D7" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="182"/>
+      <c r="C8" s="187"/>
       <c r="D8" s="82" t="s">
         <v>56</v>
       </c>
@@ -7475,7 +7543,7 @@
       <c r="C11" s="65"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="180" t="s">
+      <c r="C12" s="185" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="81" t="s">
@@ -7483,43 +7551,43 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="181"/>
+      <c r="C13" s="186"/>
       <c r="D13" s="63" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="181"/>
+      <c r="C14" s="186"/>
       <c r="D14" s="61" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="181"/>
+      <c r="C15" s="186"/>
       <c r="D15" s="80" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="181"/>
+      <c r="C16" s="186"/>
       <c r="D16" s="61" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="181"/>
+      <c r="C17" s="186"/>
       <c r="D17" s="80" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="181"/>
+      <c r="C18" s="186"/>
       <c r="D18" s="61" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="182"/>
+      <c r="C19" s="187"/>
       <c r="D19" s="82" t="s">
         <v>61</v>
       </c>

</xml_diff>